<commit_message>
Updated unit tests for AS4100_5.
</commit_message>
<xml_diff>
--- a/AS4100 Modules/Verification/Excel/AS4100_5 Verification.xlsx
+++ b/AS4100 Modules/Verification/Excel/AS4100_5 Verification.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Section Methods" sheetId="10" r:id="rId1"/>
     <sheet name="Mo" sheetId="12" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" calcMode="manual"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="66">
   <si>
     <t>Section</t>
   </si>
@@ -327,20 +327,43 @@
       <t>x</t>
     </r>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>M_o0</t>
+  </si>
+  <si>
+    <t>M_o</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="6">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="##0E+00&quot; Pa&quot;"/>
     <numFmt numFmtId="165" formatCode="##0.0000E+00&quot; m³&quot;"/>
     <numFmt numFmtId="166" formatCode="##0.00000E+00&quot; Nm&quot;"/>
     <numFmt numFmtId="167" formatCode="##0.0000E+00&quot; m&quot;"/>
     <numFmt numFmtId="168" formatCode="##0.0000E+00&quot; m⁴&quot;"/>
     <numFmt numFmtId="169" formatCode="##0.0000E+00&quot; m⁶&quot;"/>
+    <numFmt numFmtId="171" formatCode="##0.00000E+00&quot; Nm²&quot;"/>
+    <numFmt numFmtId="173" formatCode="##0.00000E+00&quot; N&quot;"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,6 +416,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -420,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -434,11 +463,41 @@
     <xf numFmtId="167" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="171" formatCode="##0.00000E+00&quot; Nm²&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -457,6 +516,206 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="167" formatCode="##0.0000E+00&quot; m&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="##0.00000E+00&quot; Nm&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="##0.00000E+00&quot; Nm&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="##0.0000E+00&quot; m&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="173" formatCode="##0.00000E+00&quot; N&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="##0.0000E+00&quot; m&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="171" formatCode="##0.00000E+00&quot; Nm²&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="##0E+00&quot; Pa&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="##0E+00&quot; Pa&quot;"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -531,31 +790,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="##0E+00&quot; Pa&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="168" formatCode="##0.0000E+00&quot; m⁴&quot;"/>
       <fill>
         <patternFill patternType="solid">
@@ -586,81 +820,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="##0E+00&quot; Pa&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="##0.00000E+00&quot; Nm&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="##0.00000E+00&quot; Nm&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -966,9 +1125,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="tblIntegral" pivot="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="22"/>
-      <tableStyleElement type="headerRow" dxfId="21"/>
-      <tableStyleElement type="secondRowStripe" dxfId="20"/>
+      <tableStyleElement type="wholeTable" dxfId="27"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
+      <tableStyleElement type="secondRowStripe" dxfId="25"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -989,17 +1148,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSection" displayName="tblSection" ref="B2:G48" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSection" displayName="tblSection" ref="B2:G48" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="B2:G48"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Section" dataDxfId="17"/>
-    <tableColumn id="2" name="Zex" dataDxfId="16"/>
-    <tableColumn id="3" name="Zey" dataDxfId="15"/>
-    <tableColumn id="13" name="fy" dataDxfId="14"/>
-    <tableColumn id="19" name="Msx" dataDxfId="13">
+    <tableColumn id="1" name="Section" dataDxfId="22"/>
+    <tableColumn id="2" name="Zex" dataDxfId="21"/>
+    <tableColumn id="3" name="Zey" dataDxfId="20"/>
+    <tableColumn id="13" name="fy" dataDxfId="19"/>
+    <tableColumn id="19" name="Msx" dataDxfId="18">
       <calculatedColumnFormula>tblSection[[#This Row],[Zex]]*tblSection[[#This Row],[fy]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="Msy" dataDxfId="12">
+    <tableColumn id="20" name="Msy" dataDxfId="17">
       <calculatedColumnFormula>tblSection[[#This Row],[Zey]]*tblSection[[#This Row],[fy]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1008,22 +1167,37 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblSection3" displayName="tblSection3" ref="B2:K48" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="B2:K48"/>
-  <tableColumns count="10">
-    <tableColumn id="1" name="Section" dataDxfId="9"/>
-    <tableColumn id="2" name="le" dataDxfId="5"/>
-    <tableColumn id="3" name="Iy" dataDxfId="4"/>
-    <tableColumn id="5" name="J" dataDxfId="2"/>
-    <tableColumn id="6" name="Iw" dataDxfId="1"/>
-    <tableColumn id="7" name="βx" dataDxfId="0"/>
-    <tableColumn id="4" name="E" dataDxfId="6"/>
-    <tableColumn id="13" name="G" dataDxfId="3"/>
-    <tableColumn id="19" name="Msx" dataDxfId="8">
-      <calculatedColumnFormula>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblM_o" displayName="tblM_o" ref="B2:P48" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="B2:P48"/>
+  <tableColumns count="15">
+    <tableColumn id="1" name="Section" dataDxfId="14"/>
+    <tableColumn id="2" name="le" dataDxfId="13"/>
+    <tableColumn id="3" name="Iy" dataDxfId="12"/>
+    <tableColumn id="5" name="J" dataDxfId="11"/>
+    <tableColumn id="6" name="Iw" dataDxfId="10"/>
+    <tableColumn id="7" name="βx" dataDxfId="1"/>
+    <tableColumn id="4" name="E" dataDxfId="9"/>
+    <tableColumn id="13" name="G" dataDxfId="8"/>
+    <tableColumn id="19" name="A" dataDxfId="5">
+      <calculatedColumnFormula>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="Msy" dataDxfId="7">
-      <calculatedColumnFormula>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</calculatedColumnFormula>
+    <tableColumn id="20" name="B" dataDxfId="7">
+      <calculatedColumnFormula>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="C" dataDxfId="0">
+      <calculatedColumnFormula>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="D0" dataDxfId="6">
+      <calculatedColumnFormula>0</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="D" dataDxfId="4">
+      <calculatedColumnFormula>tblM_o[[#This Row],[βx]]/2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" name="M_o0" dataDxfId="3">
+      <calculatedColumnFormula>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" name="M_o" dataDxfId="2">
+      <calculatedColumnFormula>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="tblIntegral" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2728,10 +2902,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M75"/>
+  <dimension ref="B1:P75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -2742,16 +2916,19 @@
     <col min="8" max="8" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" style="2" customWidth="1"/>
     <col min="10" max="11" width="16.6640625" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="2"/>
+    <col min="12" max="13" width="15.44140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="2:13" ht="11.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" ht="11.4" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2777,1033 +2954,2518 @@
         <v>55</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B3" s="1"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="10"/>
+        <v>60</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="10">
+        <v>6.7174848039124067</v>
+      </c>
+      <c r="D3" s="11">
+        <v>2.0599999999999999E-8</v>
+      </c>
+      <c r="E3" s="11">
+        <v>8.7499999999999998E-10</v>
+      </c>
+      <c r="F3" s="12">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0.1281734448884565</v>
+      </c>
       <c r="H3" s="6">
         <v>200000000000</v>
       </c>
       <c r="I3" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J3" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="10"/>
+      <c r="J3" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>901.12196558922767</v>
+      </c>
+      <c r="K3" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>70</v>
+      </c>
+      <c r="L3" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>6.408672244422825E-2</v>
+      </c>
+      <c r="O3" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>251.15440985825023</v>
+      </c>
+      <c r="P3" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>315.45830530974268</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="10">
+        <v>5.0017469968248829</v>
+      </c>
+      <c r="D4" s="11">
+        <v>3.0599999999999999E-6</v>
+      </c>
+      <c r="E4" s="11">
+        <v>1.74E-7</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10">
+        <v>-0.14231357821786134</v>
+      </c>
       <c r="H4" s="6">
         <v>200000000000</v>
       </c>
       <c r="I4" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J4" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="10"/>
+      <c r="J4" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>241439.1688792202</v>
+      </c>
+      <c r="K4" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>13920</v>
+      </c>
+      <c r="L4" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-7.1156789108930668E-2</v>
+      </c>
+      <c r="O4" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>57972.693837691761</v>
+      </c>
+      <c r="P4" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>43284.721221093743</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10">
+        <v>8.3948039770889036</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1.07E-4</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2.52E-6</v>
+      </c>
+      <c r="F5" s="12">
+        <v>2.39E-6</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0.17844856294578448</v>
+      </c>
       <c r="H5" s="6">
         <v>200000000000</v>
       </c>
       <c r="I5" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J5" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="5"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="10"/>
+      <c r="J5" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>2997039.0355725065</v>
+      </c>
+      <c r="K5" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>201600</v>
+      </c>
+      <c r="L5" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>66943.208364656923</v>
+      </c>
+      <c r="M5" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>8.9224281472892242E-2</v>
+      </c>
+      <c r="O5" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>897125.67581513233</v>
+      </c>
+      <c r="P5" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>1203539.9843339205</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="10">
+        <v>7.8809588516221565</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1.06E-7</v>
+      </c>
+      <c r="E6" s="11">
+        <v>1.9499999999999999E-8</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0.24570337922123497</v>
+      </c>
       <c r="H6" s="6">
         <v>200000000000</v>
       </c>
       <c r="I6" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J6" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="10"/>
+      <c r="J6" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>3368.8175151811124</v>
+      </c>
+      <c r="K6" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>1560</v>
+      </c>
+      <c r="L6" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>0.12285168961061749</v>
+      </c>
+      <c r="O6" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>2292.4561770473465</v>
+      </c>
+      <c r="P6" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>2743.3797871244597</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="10">
+        <v>8.158898385950641</v>
+      </c>
+      <c r="D7" s="11">
+        <v>9.7100000000000002E-5</v>
+      </c>
+      <c r="E7" s="11">
+        <v>4.0199999999999996E-6</v>
+      </c>
+      <c r="F7" s="12">
+        <v>1.15E-5</v>
+      </c>
+      <c r="G7" s="10">
+        <v>-0.14881671808883984</v>
+      </c>
       <c r="H7" s="6">
         <v>200000000000</v>
       </c>
       <c r="I7" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J7" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="10"/>
+      <c r="J7" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>2879293.4041964114</v>
+      </c>
+      <c r="K7" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>321599.99999999994</v>
+      </c>
+      <c r="L7" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>341007.9726906151</v>
+      </c>
+      <c r="M7" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-7.4408359044419919E-2</v>
+      </c>
+      <c r="O7" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>1381246.8155025893</v>
+      </c>
+      <c r="P7" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>1183520.0882903179</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="10">
+        <v>4.4411845562100432</v>
+      </c>
+      <c r="D8" s="11">
+        <v>8.6700000000000007E-5</v>
+      </c>
+      <c r="E8" s="11">
+        <v>2.9900000000000002E-6</v>
+      </c>
+      <c r="F8" s="12">
+        <v>1.34E-5</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.19001556038163414</v>
+      </c>
       <c r="H8" s="6">
         <v>200000000000</v>
       </c>
       <c r="I8" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J8" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="10"/>
+      <c r="J8" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>8676632.3688381258</v>
+      </c>
+      <c r="K8" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>239200</v>
+      </c>
+      <c r="L8" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>1341025.0720003562</v>
+      </c>
+      <c r="M8" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>9.500778019081707E-2</v>
+      </c>
+      <c r="O8" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>3702841.0727126608</v>
+      </c>
+      <c r="P8" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>4617839.5004720306</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="10">
+        <v>3.398376058418461</v>
+      </c>
+      <c r="D9" s="11">
+        <v>2.14E-4</v>
+      </c>
+      <c r="E9" s="11">
+        <v>3.0800000000000002E-6</v>
+      </c>
+      <c r="F9" s="12">
+        <v>7.3100000000000003E-6</v>
+      </c>
+      <c r="G9" s="10">
+        <v>-3.089974965237241E-2</v>
+      </c>
       <c r="H9" s="6">
         <v>200000000000</v>
       </c>
       <c r="I9" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J9" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="1"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="10"/>
+      <c r="J9" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>36576373.493588082</v>
+      </c>
+      <c r="K9" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>246400</v>
+      </c>
+      <c r="L9" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>1249407.8983090136</v>
+      </c>
+      <c r="M9" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-1.5449874826186205E-2</v>
+      </c>
+      <c r="O9" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>7396703.8850564715</v>
+      </c>
+      <c r="P9" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>6853158.6231102394</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="10">
+        <v>7.7067049543181501</v>
+      </c>
+      <c r="D10" s="11">
+        <v>1.49E-5</v>
+      </c>
+      <c r="E10" s="11">
+        <v>2.2500000000000001E-6</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.2274124460150998</v>
+      </c>
       <c r="H10" s="6">
         <v>200000000000</v>
       </c>
       <c r="I10" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J10" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="10"/>
+      <c r="J10" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>495197.61479505757</v>
+      </c>
+      <c r="K10" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>180000</v>
+      </c>
+      <c r="L10" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>0.1137062230075499</v>
+      </c>
+      <c r="O10" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>298555.8082890205</v>
+      </c>
+      <c r="P10" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>360126.16533973371</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="10">
+        <v>1.6074945841358124</v>
+      </c>
+      <c r="D11" s="11">
+        <v>7.6499999999999996E-6</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1.5699999999999999E-7</v>
+      </c>
+      <c r="F11" s="12">
+        <v>1.6500000000000001E-7</v>
+      </c>
+      <c r="G11" s="10">
+        <v>-4.3182255753713927E-2</v>
+      </c>
       <c r="H11" s="6">
         <v>200000000000</v>
       </c>
       <c r="I11" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J11" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="10"/>
+      <c r="J11" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>5843756.8783611925</v>
+      </c>
+      <c r="K11" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>12560</v>
+      </c>
+      <c r="L11" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>126041.81502347672</v>
+      </c>
+      <c r="M11" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-2.1591127876856964E-2</v>
+      </c>
+      <c r="O11" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>899975.17182241625</v>
+      </c>
+      <c r="P11" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>782603.35481326585</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.96760952227320174</v>
+      </c>
+      <c r="D12" s="11">
+        <v>1.25E-4</v>
+      </c>
+      <c r="E12" s="11">
+        <v>3.8099999999999999E-6</v>
+      </c>
+      <c r="F12" s="12">
+        <v>2.8600000000000001E-6</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0.23283024025223714</v>
+      </c>
       <c r="H12" s="6">
         <v>200000000000</v>
       </c>
       <c r="I12" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J12" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="1"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="10"/>
+      <c r="J12" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>263535719.03512019</v>
+      </c>
+      <c r="K12" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>304800</v>
+      </c>
+      <c r="L12" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>6029697.2515235497</v>
+      </c>
+      <c r="M12" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>0.11641512012611857</v>
+      </c>
+      <c r="O12" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>40857879.141069613</v>
+      </c>
+      <c r="P12" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>81773579.312149212</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="10">
+        <v>4.3986081766591001</v>
+      </c>
+      <c r="D13" s="11">
+        <v>2.6499999999999999E-8</v>
+      </c>
+      <c r="E13" s="11">
+        <v>5.5999999999999997E-9</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <v>7.8155072638581458E-2</v>
+      </c>
       <c r="H13" s="6">
         <v>200000000000</v>
       </c>
       <c r="I13" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J13" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="1"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="10"/>
+      <c r="J13" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>2703.6163276822617</v>
+      </c>
+      <c r="K13" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>448</v>
+      </c>
+      <c r="L13" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>3.9077536319290729E-2</v>
+      </c>
+      <c r="O13" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>1100.5544578991326</v>
+      </c>
+      <c r="P13" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>1211.2646023190814</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="10">
+        <v>3.6931186217914402</v>
+      </c>
+      <c r="D14" s="11">
+        <v>3.4200000000000002E-4</v>
+      </c>
+      <c r="E14" s="11">
+        <v>9.9599999999999995E-6</v>
+      </c>
+      <c r="F14" s="12">
+        <v>1.13E-4</v>
+      </c>
+      <c r="G14" s="10">
+        <v>-0.18119475342623881</v>
+      </c>
       <c r="H14" s="6">
         <v>200000000000</v>
       </c>
       <c r="I14" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J14" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="1"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="10"/>
+      <c r="J14" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>49495912.192411184</v>
+      </c>
+      <c r="K14" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>796800</v>
+      </c>
+      <c r="L14" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>16353912.508018898</v>
+      </c>
+      <c r="M14" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-9.0597376713119404E-2</v>
+      </c>
+      <c r="O14" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>29135719.663914114</v>
+      </c>
+      <c r="P14" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>24994575.752043754</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="10">
+        <v>8.8788028469425182</v>
+      </c>
+      <c r="D15" s="11">
+        <v>9.7499999999999998E-7</v>
+      </c>
+      <c r="E15" s="11">
+        <v>4.4799999999999997E-8</v>
+      </c>
+      <c r="F15" s="12">
+        <v>6.7999999999999997E-9</v>
+      </c>
+      <c r="G15" s="10">
+        <v>-0.20392675093897672</v>
+      </c>
       <c r="H15" s="6">
         <v>200000000000</v>
       </c>
       <c r="I15" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J15" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="1"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="10"/>
+      <c r="J15" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>24413.246235498838</v>
+      </c>
+      <c r="K15" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>3584</v>
+      </c>
+      <c r="L15" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>170.26674297578677</v>
+      </c>
+      <c r="M15" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-0.10196337546948836</v>
+      </c>
+      <c r="O15" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>9573.6011213133443</v>
+      </c>
+      <c r="P15" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>7402.6709695861746</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="10">
+        <v>2.649627594523889</v>
+      </c>
+      <c r="D16" s="11">
+        <v>5.2099999999999998E-4</v>
+      </c>
+      <c r="E16" s="11">
+        <v>6.37E-6</v>
+      </c>
+      <c r="F16" s="12">
+        <v>2.94E-5</v>
+      </c>
+      <c r="G16" s="10">
+        <v>6.9932775059405705E-2</v>
+      </c>
       <c r="H16" s="6">
         <v>200000000000</v>
       </c>
       <c r="I16" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J16" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="1"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="10"/>
+      <c r="J16" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>146486562.61841324</v>
+      </c>
+      <c r="K16" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>509600</v>
+      </c>
+      <c r="L16" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>8266228.2936302284</v>
+      </c>
+      <c r="M16" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>3.4966387529702853E-2</v>
+      </c>
+      <c r="O16" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>35854440.741187237</v>
+      </c>
+      <c r="P16" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>41340566.53916686</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="10">
+        <v>9.0185663204208151</v>
+      </c>
+      <c r="D17" s="11">
+        <v>5.5500000000000001E-5</v>
+      </c>
+      <c r="E17" s="11">
+        <v>5.9800000000000003E-6</v>
+      </c>
+      <c r="F17" s="12">
+        <v>6.3E-7</v>
+      </c>
+      <c r="G17" s="10">
+        <v>-0.17301834623647883</v>
+      </c>
       <c r="H17" s="6">
         <v>200000000000</v>
       </c>
       <c r="I17" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J17" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="10"/>
+      <c r="J17" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>1346938.34753423</v>
+      </c>
+      <c r="K17" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>478400</v>
+      </c>
+      <c r="L17" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>15289.570431469638</v>
+      </c>
+      <c r="M17" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-8.6509173118239413E-2</v>
+      </c>
+      <c r="O17" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>815456.56793715735</v>
+      </c>
+      <c r="P17" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>707217.0675270377</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="10">
+        <v>5.8659461348456343</v>
+      </c>
+      <c r="D18" s="11">
+        <v>1.54E-7</v>
+      </c>
+      <c r="E18" s="11">
+        <v>2E-8</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0.16142294838746213</v>
+      </c>
       <c r="H18" s="6">
         <v>200000000000</v>
       </c>
       <c r="I18" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J18" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K18" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="10"/>
+      <c r="J18" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>8834.344291413161</v>
+      </c>
+      <c r="K18" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>1600</v>
+      </c>
+      <c r="L18" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>8.0711474193731064E-2</v>
+      </c>
+      <c r="O18" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>3759.6477050730509</v>
+      </c>
+      <c r="P18" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>4539.698190885847</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="10">
+        <v>1.8597064247607875</v>
+      </c>
+      <c r="D19" s="11">
+        <v>2.97E-5</v>
+      </c>
+      <c r="E19" s="11">
+        <v>3.4499999999999998E-7</v>
+      </c>
+      <c r="F19" s="12">
+        <v>4.15E-7</v>
+      </c>
+      <c r="G19" s="10">
+        <v>-0.17861962325821534</v>
+      </c>
       <c r="H19" s="6">
         <v>200000000000</v>
       </c>
       <c r="I19" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J19" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="1"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="10"/>
+      <c r="J19" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>16951081.326039746</v>
+      </c>
+      <c r="K19" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>27600</v>
+      </c>
+      <c r="L19" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>236858.54378136346</v>
+      </c>
+      <c r="M19" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-8.9309811629107672E-2</v>
+      </c>
+      <c r="O19" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>2117276.1470823628</v>
+      </c>
+      <c r="P19" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>1088936.1665291372</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="10">
+        <v>3.1958853402372531</v>
+      </c>
+      <c r="D20" s="11">
+        <v>4.6900000000000001E-9</v>
+      </c>
+      <c r="E20" s="11">
+        <v>1.6600000000000001E-9</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="10">
+        <v>-0.11678148562170115</v>
+      </c>
       <c r="H20" s="6">
         <v>200000000000</v>
       </c>
       <c r="I20" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J20" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K20" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="1"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="10"/>
+      <c r="J20" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>906.40064219555916</v>
+      </c>
+      <c r="K20" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>132.80000000000001</v>
+      </c>
+      <c r="L20" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-5.8390742810850577E-2</v>
+      </c>
+      <c r="O20" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>346.94380709787896</v>
+      </c>
+      <c r="P20" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>298.03200369196639</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="10">
+        <v>9.1955411751463512</v>
+      </c>
+      <c r="D21" s="11">
+        <v>4.0400000000000003E-6</v>
+      </c>
+      <c r="E21" s="11">
+        <v>2.8999999999999998E-7</v>
+      </c>
+      <c r="F21" s="12">
+        <v>5.8199999999999998E-8</v>
+      </c>
+      <c r="G21" s="10">
+        <v>4.8268222412633233E-2</v>
+      </c>
       <c r="H21" s="6">
         <v>200000000000</v>
       </c>
       <c r="I21" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J21" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K21" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="1"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="10"/>
+      <c r="J21" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>94309.733883130044</v>
+      </c>
+      <c r="K21" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>23199.999999999996</v>
+      </c>
+      <c r="L21" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>1358.6204237619229</v>
+      </c>
+      <c r="M21" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>2.4134111206316616E-2</v>
+      </c>
+      <c r="O21" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>48126.05278538631</v>
+      </c>
+      <c r="P21" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>50455.92701998767</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="10">
+        <v>2.2710216302220676</v>
+      </c>
+      <c r="D22" s="11">
+        <v>2.8600000000000001E-4</v>
+      </c>
+      <c r="E22" s="11">
+        <v>1.6500000000000001E-5</v>
+      </c>
+      <c r="F22" s="12">
+        <v>7.0999999999999998E-6</v>
+      </c>
+      <c r="G22" s="10">
+        <v>-0.12280782830035036</v>
+      </c>
       <c r="H22" s="6">
         <v>200000000000</v>
       </c>
       <c r="I22" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J22" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K22" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="1"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="10"/>
+      <c r="J22" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>109459442.75587614</v>
+      </c>
+      <c r="K22" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>1320000</v>
+      </c>
+      <c r="L22" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>2717349.8026808412</v>
+      </c>
+      <c r="M22" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-6.1403914150175182E-2</v>
+      </c>
+      <c r="O22" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>21022037.475277971</v>
+      </c>
+      <c r="P22" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>15349128.850817373</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="10">
+        <v>1.0215889232004904</v>
+      </c>
+      <c r="D23" s="11">
+        <v>9.0199999999999997E-5</v>
+      </c>
+      <c r="E23" s="11">
+        <v>1.6300000000000001E-6</v>
+      </c>
+      <c r="F23" s="12">
+        <v>1.9800000000000001E-6</v>
+      </c>
+      <c r="G23" s="10">
+        <v>4.071375607714639E-2</v>
+      </c>
       <c r="H23" s="6">
         <v>200000000000</v>
       </c>
       <c r="I23" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J23" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K23" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="1"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="10"/>
+      <c r="J23" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>170601925.25226769</v>
+      </c>
+      <c r="K23" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>130400</v>
+      </c>
+      <c r="L23" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>3744920.3104156326</v>
+      </c>
+      <c r="M23" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>2.0356878038573195E-2</v>
+      </c>
+      <c r="O23" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>25712586.527343422</v>
+      </c>
+      <c r="P23" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>29418987.744043078</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="10">
+        <v>9.1350130430458663</v>
+      </c>
+      <c r="D24" s="11">
+        <v>1.73E-6</v>
+      </c>
+      <c r="E24" s="11">
+        <v>1.4100000000000001E-7</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="10">
+        <v>6.1145604051748181E-2</v>
+      </c>
       <c r="H24" s="6">
         <v>200000000000</v>
       </c>
       <c r="I24" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J24" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="1"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="10"/>
+      <c r="J24" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>40922.061208469393</v>
+      </c>
+      <c r="K24" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>11280</v>
+      </c>
+      <c r="L24" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>3.0572802025874091E-2</v>
+      </c>
+      <c r="O24" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>21484.898194581579</v>
+      </c>
+      <c r="P24" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>22772.396340699379</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="10">
+        <v>7.7754643459347816</v>
+      </c>
+      <c r="D25" s="11">
+        <v>5.8500000000000001E-7</v>
+      </c>
+      <c r="E25" s="11">
+        <v>1.1000000000000001E-7</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0</v>
+      </c>
+      <c r="G25" s="10">
+        <v>0.21295192832515658</v>
+      </c>
       <c r="H25" s="6">
         <v>200000000000</v>
       </c>
       <c r="I25" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J25" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K25" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="1"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="10"/>
+      <c r="J25" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>19099.981147935767</v>
+      </c>
+      <c r="K25" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>8800</v>
+      </c>
+      <c r="L25" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>0.10647596416257829</v>
+      </c>
+      <c r="O25" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>12964.560698374424</v>
+      </c>
+      <c r="P25" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>15156.78780585297</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="10">
+        <v>3.7318328934894165</v>
+      </c>
+      <c r="D26" s="11">
+        <v>2.5500000000000001E-6</v>
+      </c>
+      <c r="E26" s="11">
+        <v>6.7399999999999995E-8</v>
+      </c>
+      <c r="F26" s="12">
+        <v>3.6699999999999998E-8</v>
+      </c>
+      <c r="G26" s="10">
+        <v>-0.12592274557462746</v>
+      </c>
       <c r="H26" s="6">
         <v>200000000000</v>
       </c>
       <c r="I26" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J26" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K26" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="1"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="10"/>
+      <c r="J26" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>361431.12099591718</v>
+      </c>
+      <c r="K26" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>5392</v>
+      </c>
+      <c r="L26" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>5201.7733884510417</v>
+      </c>
+      <c r="M26" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-6.296137278731373E-2</v>
+      </c>
+      <c r="O26" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>61878.262672481171</v>
+      </c>
+      <c r="P26" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>43173.793697935238</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="10">
+        <v>7.005314481683639</v>
+      </c>
+      <c r="D27" s="11">
+        <v>4.1999999999999998E-5</v>
+      </c>
+      <c r="E27" s="11">
+        <v>8.2699999999999998E-7</v>
+      </c>
+      <c r="F27" s="12">
+        <v>6.0299999999999999E-7</v>
+      </c>
+      <c r="G27" s="10">
+        <v>-3.8294633993238014E-2</v>
+      </c>
       <c r="H27" s="6">
         <v>200000000000</v>
       </c>
       <c r="I27" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J27" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K27" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="1"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="10"/>
+      <c r="J27" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>1689366.0364728088</v>
+      </c>
+      <c r="K27" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>66160</v>
+      </c>
+      <c r="L27" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>24254.469523645326</v>
+      </c>
+      <c r="M27" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-1.9147316996619007E-2</v>
+      </c>
+      <c r="O27" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>390823.66102751798</v>
+      </c>
+      <c r="P27" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>359813.15466422978</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="10">
+        <v>6.7881422970076946</v>
+      </c>
+      <c r="D28" s="11">
+        <v>8.5700000000000001E-7</v>
+      </c>
+      <c r="E28" s="11">
+        <v>1.1000000000000001E-7</v>
+      </c>
+      <c r="F28" s="12">
+        <v>0</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0.11489505543493223</v>
+      </c>
       <c r="H28" s="6">
         <v>200000000000</v>
       </c>
       <c r="I28" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J28" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="1"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="10"/>
+      <c r="J28" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>36712.05434911645</v>
+      </c>
+      <c r="K28" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>8800</v>
+      </c>
+      <c r="L28" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>5.7447527717466113E-2</v>
+      </c>
+      <c r="O28" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>17974.039008309312</v>
+      </c>
+      <c r="P28" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>20206.365459672474</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="10">
+        <v>7.9035087500929846</v>
+      </c>
+      <c r="D29" s="11">
+        <v>9.3600000000000004E-8</v>
+      </c>
+      <c r="E29" s="11">
+        <v>1.7599999999999999E-8</v>
+      </c>
+      <c r="F29" s="12">
+        <v>0</v>
+      </c>
+      <c r="G29" s="10">
+        <v>-8.7427357914032777E-3</v>
+      </c>
       <c r="H29" s="6">
         <v>200000000000</v>
       </c>
       <c r="I29" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J29" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K29" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="1"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="10"/>
+      <c r="J29" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>2957.7789437803704</v>
+      </c>
+      <c r="K29" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>1408</v>
+      </c>
+      <c r="L29" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-4.3713678957016389E-3</v>
+      </c>
+      <c r="O29" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>2040.7235856045675</v>
+      </c>
+      <c r="P29" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>2027.8350045230263</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="10">
+        <v>1.0861476712532603</v>
+      </c>
+      <c r="D30" s="11">
+        <v>1.2899999999999999E-6</v>
+      </c>
+      <c r="E30" s="11">
+        <v>5.4900000000000002E-8</v>
+      </c>
+      <c r="F30" s="12">
+        <v>4.5900000000000001E-9</v>
+      </c>
+      <c r="G30" s="10">
+        <v>-0.17344979293160129</v>
+      </c>
       <c r="H30" s="6">
         <v>200000000000</v>
       </c>
       <c r="I30" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J30" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K30" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="10"/>
+      <c r="J30" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>2158448.5477226921</v>
+      </c>
+      <c r="K30" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>4392</v>
+      </c>
+      <c r="L30" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>7680.0611116644641</v>
+      </c>
+      <c r="M30" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-8.6724896465800644E-2</v>
+      </c>
+      <c r="O30" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>161421.56849223017</v>
+      </c>
+      <c r="P30" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>59987.813901311281</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="10">
+        <v>9.5844968325732616</v>
+      </c>
+      <c r="D31" s="11">
+        <v>1.6500000000000001E-6</v>
+      </c>
+      <c r="E31" s="11">
+        <v>1.01E-7</v>
+      </c>
+      <c r="F31" s="12">
+        <v>1.0600000000000001E-8</v>
+      </c>
+      <c r="G31" s="10">
+        <v>0.23509132247412962</v>
+      </c>
       <c r="H31" s="6">
         <v>200000000000</v>
       </c>
       <c r="I31" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J31" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K31" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="10"/>
+      <c r="J31" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>35454.800734916906</v>
+      </c>
+      <c r="K31" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>8080</v>
+      </c>
+      <c r="L31" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>227.77023502431467</v>
+      </c>
+      <c r="M31" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>0.11754566123706481</v>
+      </c>
+      <c r="O31" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>17162.468885165119</v>
+      </c>
+      <c r="P31" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>21828.783262169007</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="10">
+        <v>5.6367905253762451</v>
+      </c>
+      <c r="D32" s="11">
+        <v>3.8800000000000001E-5</v>
+      </c>
+      <c r="E32" s="11">
+        <v>5.8599999999999998E-7</v>
+      </c>
+      <c r="F32" s="12">
+        <v>5.5700000000000002E-7</v>
+      </c>
+      <c r="G32" s="10">
+        <v>1.8946619081317728E-2</v>
+      </c>
       <c r="H32" s="6">
         <v>200000000000</v>
       </c>
       <c r="I32" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J32" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K32" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="1"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="10"/>
+      <c r="J32" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>2410447.4890987067</v>
+      </c>
+      <c r="K32" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>46880</v>
+      </c>
+      <c r="L32" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>34603.588954329374</v>
+      </c>
+      <c r="M32" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>9.4733095406588641E-3</v>
+      </c>
+      <c r="O32" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>443183.83589399373</v>
+      </c>
+      <c r="P32" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>466606.64226913889</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="10">
+        <v>2.3688223785605809</v>
+      </c>
+      <c r="D33" s="11">
+        <v>7.2899999999999997E-5</v>
+      </c>
+      <c r="E33" s="11">
+        <v>9.2800000000000005E-7</v>
+      </c>
+      <c r="F33" s="12">
+        <v>1.5600000000000001E-6</v>
+      </c>
+      <c r="G33" s="10">
+        <v>0.14839370809904429</v>
+      </c>
       <c r="H33" s="6">
         <v>200000000000</v>
       </c>
       <c r="I33" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J33" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K33" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="10"/>
+      <c r="J33" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>25644384.206543483</v>
+      </c>
+      <c r="K33" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>74240</v>
+      </c>
+      <c r="L33" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>548768.71553097165</v>
+      </c>
+      <c r="M33" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>7.4196854049522143E-2</v>
+      </c>
+      <c r="O33" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>3997083.2947414783</v>
+      </c>
+      <c r="P33" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>6329590.0202653678</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="10">
+        <v>1.1862405919482266</v>
+      </c>
+      <c r="D34" s="11">
+        <v>1.7100000000000001E-4</v>
+      </c>
+      <c r="E34" s="11">
+        <v>1.5799999999999999E-6</v>
+      </c>
+      <c r="F34" s="12">
+        <v>5.7200000000000003E-6</v>
+      </c>
+      <c r="G34" s="10">
+        <v>-0.24494910732988207</v>
+      </c>
       <c r="H34" s="6">
         <v>200000000000</v>
       </c>
       <c r="I34" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J34" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K34" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B35" s="1"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="10"/>
+      <c r="J34" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>239872404.91553012</v>
+      </c>
+      <c r="K34" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>126399.99999999999</v>
+      </c>
+      <c r="L34" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>8023802.0825545741</v>
+      </c>
+      <c r="M34" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N34" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-0.12247455366494103</v>
+      </c>
+      <c r="O34" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>44215478.896987282</v>
+      </c>
+      <c r="P34" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>23707429.814660929</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="10">
+        <v>7.1494209501459469</v>
+      </c>
+      <c r="D35" s="11">
+        <v>3.03E-8</v>
+      </c>
+      <c r="E35" s="11">
+        <v>2.9600000000000001E-9</v>
+      </c>
+      <c r="F35" s="12">
+        <v>0</v>
+      </c>
+      <c r="G35" s="10">
+        <v>0.13268382903565945</v>
+      </c>
       <c r="H35" s="6">
         <v>200000000000</v>
       </c>
       <c r="I35" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J35" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K35" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B36" s="1"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="10"/>
+      <c r="J35" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>1170.1206192996688</v>
+      </c>
+      <c r="K35" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>236.8</v>
+      </c>
+      <c r="L35" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>6.6341914517829725E-2</v>
+      </c>
+      <c r="O35" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>526.38822427003595</v>
+      </c>
+      <c r="P35" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>609.70949786764584</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="10">
+        <v>0.92837068195856243</v>
+      </c>
+      <c r="D36" s="11">
+        <v>4.2700000000000002E-4</v>
+      </c>
+      <c r="E36" s="11">
+        <v>1.9199999999999999E-5</v>
+      </c>
+      <c r="F36" s="12">
+        <v>1.6200000000000001E-5</v>
+      </c>
+      <c r="G36" s="10">
+        <v>8.9370921465537101E-2</v>
+      </c>
       <c r="H36" s="6">
         <v>200000000000</v>
       </c>
       <c r="I36" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J36" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K36" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="10"/>
+      <c r="J36" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>977945791.77435112</v>
+      </c>
+      <c r="K36" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>1536000</v>
+      </c>
+      <c r="L36" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>37102393.036872342</v>
+      </c>
+      <c r="M36" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>4.468546073276855E-2</v>
+      </c>
+      <c r="O36" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>194386866.50937274</v>
+      </c>
+      <c r="P36" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>242938358.75441101</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="10">
+        <v>8.3148258094870968</v>
+      </c>
+      <c r="D37" s="11">
+        <v>3.93E-5</v>
+      </c>
+      <c r="E37" s="11">
+        <v>1.5600000000000001E-6</v>
+      </c>
+      <c r="F37" s="12">
+        <v>3.45E-6</v>
+      </c>
+      <c r="G37" s="10">
+        <v>4.729885293709063E-2</v>
+      </c>
       <c r="H37" s="6">
         <v>200000000000</v>
       </c>
       <c r="I37" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J37" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K37" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38" s="1"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="10"/>
+      <c r="J37" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>1122059.7414560022</v>
+      </c>
+      <c r="K37" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>124800.00000000001</v>
+      </c>
+      <c r="L37" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>98501.427685068906</v>
+      </c>
+      <c r="M37" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>2.3649426468545315E-2</v>
+      </c>
+      <c r="O37" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>500557.23170788836</v>
+      </c>
+      <c r="P37" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>527796.18664483225</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="10">
+        <v>4.033202377994817</v>
+      </c>
+      <c r="D38" s="11">
+        <v>2.8200000000000001E-7</v>
+      </c>
+      <c r="E38" s="11">
+        <v>4.1899999999999998E-8</v>
+      </c>
+      <c r="F38" s="12">
+        <v>0</v>
+      </c>
+      <c r="G38" s="10">
+        <v>-4.3008266672655227E-2</v>
+      </c>
       <c r="H38" s="6">
         <v>200000000000</v>
       </c>
       <c r="I38" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J38" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K38" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="1"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="10"/>
+      <c r="J38" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>34219.906629327801</v>
+      </c>
+      <c r="K38" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>3352</v>
+      </c>
+      <c r="L38" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-2.1504133336327613E-2</v>
+      </c>
+      <c r="O38" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>10710.047946741732</v>
+      </c>
+      <c r="P38" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>9999.4289236204531</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="10">
+        <v>8.6844874800771716</v>
+      </c>
+      <c r="D39" s="11">
+        <v>1.1400000000000001E-6</v>
+      </c>
+      <c r="E39" s="11">
+        <v>3.8600000000000002E-8</v>
+      </c>
+      <c r="F39" s="12">
+        <v>1.04E-8</v>
+      </c>
+      <c r="G39" s="10">
+        <v>-0.14461917695438892</v>
+      </c>
       <c r="H39" s="6">
         <v>200000000000</v>
       </c>
       <c r="I39" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J39" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K39" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="1"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="10"/>
+      <c r="J39" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>29836.385209670414</v>
+      </c>
+      <c r="K39" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>3088</v>
+      </c>
+      <c r="L39" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>272.19158436892303</v>
+      </c>
+      <c r="M39" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-7.2309588477194459E-2</v>
+      </c>
+      <c r="O39" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>10012.790344830153</v>
+      </c>
+      <c r="P39" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>8085.1303422081046</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="10">
+        <v>3.6053619609274556</v>
+      </c>
+      <c r="D40" s="11">
+        <v>1.1800000000000001E-5</v>
+      </c>
+      <c r="E40" s="11">
+        <v>1.06E-6</v>
+      </c>
+      <c r="F40" s="12">
+        <v>0</v>
+      </c>
+      <c r="G40" s="10">
+        <v>4.5483544252193642E-2</v>
+      </c>
       <c r="H40" s="6">
         <v>200000000000</v>
       </c>
       <c r="I40" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J40" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K40" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="1"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="10"/>
+      <c r="J40" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>1791900.9665836114</v>
+      </c>
+      <c r="K40" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>84800</v>
+      </c>
+      <c r="L40" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M40" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N40" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>2.2741772126096821E-2</v>
+      </c>
+      <c r="O40" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>389811.75196021254</v>
+      </c>
+      <c r="P40" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>432687.02661249664</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="10">
+        <v>8.1094334587245278</v>
+      </c>
+      <c r="D41" s="11">
+        <v>5.8700000000000003E-8</v>
+      </c>
+      <c r="E41" s="11">
+        <v>3.8700000000000001E-9</v>
+      </c>
+      <c r="F41" s="12">
+        <v>0</v>
+      </c>
+      <c r="G41" s="10">
+        <v>-0.1313367378988039</v>
+      </c>
       <c r="H41" s="6">
         <v>200000000000</v>
       </c>
       <c r="I41" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J41" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K41" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="10"/>
+      <c r="J41" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>1761.9225467519443</v>
+      </c>
+      <c r="K41" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>309.60000000000002</v>
+      </c>
+      <c r="L41" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M41" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N41" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-6.5668368949401951E-2</v>
+      </c>
+      <c r="O41" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>738.57377456446557</v>
+      </c>
+      <c r="P41" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>631.87905946789692</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="10">
+        <v>3.0434412324018068</v>
+      </c>
+      <c r="D42" s="11">
+        <v>4.1699999999999997E-5</v>
+      </c>
+      <c r="E42" s="11">
+        <v>9.2099999999999995E-7</v>
+      </c>
+      <c r="F42" s="12">
+        <v>6.28E-6</v>
+      </c>
+      <c r="G42" s="10">
+        <v>5.1439072240297534E-2</v>
+      </c>
       <c r="H42" s="6">
         <v>200000000000</v>
       </c>
       <c r="I42" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J42" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K42" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B43" s="1"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="10"/>
+      <c r="J42" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>8886606.6186649669</v>
+      </c>
+      <c r="K42" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>73680</v>
+      </c>
+      <c r="L42" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>1338318.6946094965</v>
+      </c>
+      <c r="M42" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N42" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>2.5719536120148767E-2</v>
+      </c>
+      <c r="O42" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>3542298.2574965428</v>
+      </c>
+      <c r="P42" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>3778223.6578902965</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="10">
+        <v>4.539654505580625</v>
+      </c>
+      <c r="D43" s="11">
+        <v>6.6600000000000001E-8</v>
+      </c>
+      <c r="E43" s="11">
+        <v>4.32E-9</v>
+      </c>
+      <c r="F43" s="12">
+        <v>0</v>
+      </c>
+      <c r="G43" s="10">
+        <v>-0.13004473881389744</v>
+      </c>
       <c r="H43" s="6">
         <v>200000000000</v>
       </c>
       <c r="I43" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J43" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K43" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B44" s="1"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="10"/>
+      <c r="J43" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>6379.0846717143495</v>
+      </c>
+      <c r="K43" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>345.6</v>
+      </c>
+      <c r="L43" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M43" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N43" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-6.5022369406948721E-2</v>
+      </c>
+      <c r="O43" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>1484.7934747110385</v>
+      </c>
+      <c r="P43" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>1126.8577327535636</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="10">
+        <v>9.0047283243181671</v>
+      </c>
+      <c r="D44" s="11">
+        <v>5.82E-7</v>
+      </c>
+      <c r="E44" s="11">
+        <v>3.1699999999999999E-8</v>
+      </c>
+      <c r="F44" s="12">
+        <v>0</v>
+      </c>
+      <c r="G44" s="10">
+        <v>-8.562069737511574E-2</v>
+      </c>
       <c r="H44" s="6">
         <v>200000000000</v>
       </c>
       <c r="I44" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J44" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K44" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B45" s="1"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="10"/>
+      <c r="J44" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>14168.096187192119</v>
+      </c>
+      <c r="K44" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>2536</v>
+      </c>
+      <c r="L44" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M44" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N44" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-4.281034868755787E-2</v>
+      </c>
+      <c r="O44" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>5994.1881794550982</v>
+      </c>
+      <c r="P44" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>5418.2562928410998</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="10">
+        <v>1.0580889776533575</v>
+      </c>
+      <c r="D45" s="11">
+        <v>3.3700000000000001E-7</v>
+      </c>
+      <c r="E45" s="11">
+        <v>4.0200000000000003E-8</v>
+      </c>
+      <c r="F45" s="12">
+        <v>1.14E-9</v>
+      </c>
+      <c r="G45" s="10">
+        <v>-0.13883820036535327</v>
+      </c>
       <c r="H45" s="6">
         <v>200000000000</v>
       </c>
       <c r="I45" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J45" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K45" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B46" s="1"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="10"/>
+      <c r="J45" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>594176.21290671604</v>
+      </c>
+      <c r="K45" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>3216</v>
+      </c>
+      <c r="L45" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>2009.9729457378526</v>
+      </c>
+      <c r="M45" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N45" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>-6.9419100182676635E-2</v>
+      </c>
+      <c r="O45" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>55723.862156633331</v>
+      </c>
+      <c r="P45" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>28081.593111355083</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="10">
+        <v>8.2944829261764603</v>
+      </c>
+      <c r="D46" s="11">
+        <v>8.34E-4</v>
+      </c>
+      <c r="E46" s="11">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="F46" s="12">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="G46" s="10">
+        <v>8.2085432298504346E-2</v>
+      </c>
       <c r="H46" s="6">
         <v>200000000000</v>
       </c>
       <c r="I46" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J46" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K46" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B47" s="1"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="10"/>
+      <c r="J46" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>23928592.658485726</v>
+      </c>
+      <c r="K46" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>1760000</v>
+      </c>
+      <c r="L46" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>8033580.2690359745</v>
+      </c>
+      <c r="M46" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N46" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>4.1042716149252173E-2</v>
+      </c>
+      <c r="O46" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>15308383.093127273</v>
+      </c>
+      <c r="P46" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>16321947.83875609</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="10">
+        <v>2.8892682314493143</v>
+      </c>
+      <c r="D47" s="11">
+        <v>9.0100000000000001E-6</v>
+      </c>
+      <c r="E47" s="11">
+        <v>2.3300000000000001E-7</v>
+      </c>
+      <c r="F47" s="12">
+        <v>1.97E-7</v>
+      </c>
+      <c r="G47" s="10">
+        <v>0.11020676524520689</v>
+      </c>
       <c r="H47" s="6">
         <v>200000000000</v>
       </c>
       <c r="I47" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J47" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K47" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B48" s="1"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="10"/>
+      <c r="J47" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>2130486.6013809559</v>
+      </c>
+      <c r="K47" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>18640</v>
+      </c>
+      <c r="L47" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>46582.22646748594</v>
+      </c>
+      <c r="M47" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N47" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>5.5103382622603447E-2</v>
+      </c>
+      <c r="O47" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>372766.78983140807</v>
+      </c>
+      <c r="P47" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>508213.01026589843</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" s="10">
+        <v>6.1787388734517847</v>
+      </c>
+      <c r="D48" s="11">
+        <v>1.8699999999999999E-7</v>
+      </c>
+      <c r="E48" s="11">
+        <v>1.1199999999999999E-8</v>
+      </c>
+      <c r="F48" s="12">
+        <v>0</v>
+      </c>
+      <c r="G48" s="10">
+        <v>0.18629697564513525</v>
+      </c>
       <c r="H48" s="6">
         <v>200000000000</v>
       </c>
       <c r="I48" s="6">
         <v>80000000000</v>
       </c>
-      <c r="J48" s="9">
-        <f>tblSection3[[#This Row],[le]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
-      </c>
-      <c r="K48" s="9">
-        <f>tblSection3[[#This Row],[Iy]]*tblSection3[[#This Row],[G]]</f>
-        <v>0</v>
+      <c r="J48" s="16">
+        <f>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</f>
+        <v>9668.7796933411191</v>
+      </c>
+      <c r="K48" s="14">
+        <f>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</f>
+        <v>896</v>
+      </c>
+      <c r="L48" s="14">
+        <f>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="M48" s="15">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N48" s="15">
+        <f>tblM_o[[#This Row],[βx]]/2</f>
+        <v>9.3148487822567627E-2</v>
+      </c>
+      <c r="O48" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>2943.3359654028018</v>
+      </c>
+      <c r="P48" s="17">
+        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <v>3978.6778502111547</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="str">
-        <f t="array" ref="B50:B75">TRANSPOSE(tblSection3[#Headers])</f>
+        <f t="array" ref="B50:B75">TRANSPOSE(tblM_o[#Headers])</f>
         <v>Section</v>
       </c>
       <c r="C50" s="4" t="str">
-        <f t="array" aca="1" ref="C50" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B50&amp;"]")&lt;&gt;"","'"&amp;TEXT(INDIRECT("tblSection["&amp;B50&amp;"]"),"0.00000E+00")&amp;"', ",""))</f>
+        <f t="array" aca="1" ref="C50" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B50&amp;"]")&lt;&gt;"","'"&amp;TEXT(INDIRECT("tblM_o["&amp;B50&amp;"]"),"0.00000E+00")&amp;"', ",""))</f>
         <v xml:space="preserve">'45x45x3EA', '150x150x12EA', '310UC137', '75x50x8UA', '700WB173', '800WB168', '400WC181', '200x200x26EA', '310UB40.4', '310UC158', '40x40x6EA', '1200WB342', '180UB18.1', '500WC267', '200UBP146', '65x65x8EA', '250UBP62.6', '25x25x5EA', '300PFC', '350WC280', '310UC118', '125x125x12EA', '125x75x12UA', '250UB25.7', '250UBP84.9', '100x100x12EA', '65x50x8UA', '150PFC', '200PFC', '250UC72.9', '310UC96.8', '400WC144', '45x45x5EA', '400WC328', '610UB125', '75x75x10EA', '200UB18.2', '200x200x20EA', '65x50x5UA', '800WB122', '75x50x5UA', '100x100x8EA', '125TFB', '1200WB455', '310UB46.2', '75x75x6EA', </v>
       </c>
       <c r="D50" s="2" t="str">
@@ -3815,182 +5477,182 @@
       <c r="B51" s="2" t="str">
         <v>le</v>
       </c>
-      <c r="C51" s="4" t="e">
-        <f t="array" aca="1" ref="C51" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B51&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B51&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D51" s="2" t="e">
+      <c r="C51" s="4" t="str">
+        <f t="array" aca="1" ref="C51" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B51&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B51&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">6.71748E+00, 5.00175E+00, 8.39480E+00, 7.88096E+00, 8.15890E+00, 4.44118E+00, 3.39838E+00, 7.70670E+00, 1.60749E+00, 9.67610E-01, 4.39861E+00, 3.69312E+00, 8.87880E+00, 2.64963E+00, 9.01857E+00, 5.86595E+00, 1.85971E+00, 3.19589E+00, 9.19554E+00, 2.27102E+00, 1.02159E+00, 9.13501E+00, 7.77546E+00, 3.73183E+00, 7.00531E+00, 6.78814E+00, 7.90351E+00, 1.08615E+00, 9.58450E+00, 5.63679E+00, 2.36882E+00, 1.18624E+00, 7.14942E+00, 9.28371E-01, 8.31483E+00, 4.03320E+00, 8.68449E+00, 3.60536E+00, 8.10943E+00, 3.04344E+00, 4.53965E+00, 9.00473E+00, 1.05809E+00, 8.29448E+00, 2.88927E+00, 6.17874E+00, </v>
+      </c>
+      <c r="D51" s="2" t="str">
         <f t="shared" ref="D51:D75" ca="1" si="0">B51&amp;" = ("&amp;LEFT(C51,LEN(C51)-2)&amp;")"</f>
-        <v>#REF!</v>
+        <v>le = (6.71748E+00, 5.00175E+00, 8.39480E+00, 7.88096E+00, 8.15890E+00, 4.44118E+00, 3.39838E+00, 7.70670E+00, 1.60749E+00, 9.67610E-01, 4.39861E+00, 3.69312E+00, 8.87880E+00, 2.64963E+00, 9.01857E+00, 5.86595E+00, 1.85971E+00, 3.19589E+00, 9.19554E+00, 2.27102E+00, 1.02159E+00, 9.13501E+00, 7.77546E+00, 3.73183E+00, 7.00531E+00, 6.78814E+00, 7.90351E+00, 1.08615E+00, 9.58450E+00, 5.63679E+00, 2.36882E+00, 1.18624E+00, 7.14942E+00, 9.28371E-01, 8.31483E+00, 4.03320E+00, 8.68449E+00, 3.60536E+00, 8.10943E+00, 3.04344E+00, 4.53965E+00, 9.00473E+00, 1.05809E+00, 8.29448E+00, 2.88927E+00, 6.17874E+00)</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="str">
         <v>Iy</v>
       </c>
-      <c r="C52" s="4" t="e">
-        <f t="array" aca="1" ref="C52" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B52&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B52&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D52" s="2" t="e">
+      <c r="C52" s="4" t="str">
+        <f t="array" aca="1" ref="C52" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B52&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B52&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">2.06000E-08, 3.06000E-06, 1.07000E-04, 1.06000E-07, 9.71000E-05, 8.67000E-05, 2.14000E-04, 1.49000E-05, 7.65000E-06, 1.25000E-04, 2.65000E-08, 3.42000E-04, 9.75000E-07, 5.21000E-04, 5.55000E-05, 1.54000E-07, 2.97000E-05, 4.69000E-09, 4.04000E-06, 2.86000E-04, 9.02000E-05, 1.73000E-06, 5.85000E-07, 2.55000E-06, 4.20000E-05, 8.57000E-07, 9.36000E-08, 1.29000E-06, 1.65000E-06, 3.88000E-05, 7.29000E-05, 1.71000E-04, 3.03000E-08, 4.27000E-04, 3.93000E-05, 2.82000E-07, 1.14000E-06, 1.18000E-05, 5.87000E-08, 4.17000E-05, 6.66000E-08, 5.82000E-07, 3.37000E-07, 8.34000E-04, 9.01000E-06, 1.87000E-07, </v>
+      </c>
+      <c r="D52" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>#REF!</v>
+        <v>Iy = (2.06000E-08, 3.06000E-06, 1.07000E-04, 1.06000E-07, 9.71000E-05, 8.67000E-05, 2.14000E-04, 1.49000E-05, 7.65000E-06, 1.25000E-04, 2.65000E-08, 3.42000E-04, 9.75000E-07, 5.21000E-04, 5.55000E-05, 1.54000E-07, 2.97000E-05, 4.69000E-09, 4.04000E-06, 2.86000E-04, 9.02000E-05, 1.73000E-06, 5.85000E-07, 2.55000E-06, 4.20000E-05, 8.57000E-07, 9.36000E-08, 1.29000E-06, 1.65000E-06, 3.88000E-05, 7.29000E-05, 1.71000E-04, 3.03000E-08, 4.27000E-04, 3.93000E-05, 2.82000E-07, 1.14000E-06, 1.18000E-05, 5.87000E-08, 4.17000E-05, 6.66000E-08, 5.82000E-07, 3.37000E-07, 8.34000E-04, 9.01000E-06, 1.87000E-07)</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="str">
         <v>J</v>
       </c>
-      <c r="C53" s="4" t="e">
-        <f t="array" aca="1" ref="C53" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B53&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B53&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D53" s="2" t="e">
+      <c r="C53" s="4" t="str">
+        <f t="array" aca="1" ref="C53" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B53&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B53&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">8.75000E-10, 1.74000E-07, 2.52000E-06, 1.95000E-08, 4.02000E-06, 2.99000E-06, 3.08000E-06, 2.25000E-06, 1.57000E-07, 3.81000E-06, 5.60000E-09, 9.96000E-06, 4.48000E-08, 6.37000E-06, 5.98000E-06, 2.00000E-08, 3.45000E-07, 1.66000E-09, 2.90000E-07, 1.65000E-05, 1.63000E-06, 1.41000E-07, 1.10000E-07, 6.74000E-08, 8.27000E-07, 1.10000E-07, 1.76000E-08, 5.49000E-08, 1.01000E-07, 5.86000E-07, 9.28000E-07, 1.58000E-06, 2.96000E-09, 1.92000E-05, 1.56000E-06, 4.19000E-08, 3.86000E-08, 1.06000E-06, 3.87000E-09, 9.21000E-07, 4.32000E-09, 3.17000E-08, 4.02000E-08, 2.20000E-05, 2.33000E-07, 1.12000E-08, </v>
+      </c>
+      <c r="D53" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>#REF!</v>
+        <v>J = (8.75000E-10, 1.74000E-07, 2.52000E-06, 1.95000E-08, 4.02000E-06, 2.99000E-06, 3.08000E-06, 2.25000E-06, 1.57000E-07, 3.81000E-06, 5.60000E-09, 9.96000E-06, 4.48000E-08, 6.37000E-06, 5.98000E-06, 2.00000E-08, 3.45000E-07, 1.66000E-09, 2.90000E-07, 1.65000E-05, 1.63000E-06, 1.41000E-07, 1.10000E-07, 6.74000E-08, 8.27000E-07, 1.10000E-07, 1.76000E-08, 5.49000E-08, 1.01000E-07, 5.86000E-07, 9.28000E-07, 1.58000E-06, 2.96000E-09, 1.92000E-05, 1.56000E-06, 4.19000E-08, 3.86000E-08, 1.06000E-06, 3.87000E-09, 9.21000E-07, 4.32000E-09, 3.17000E-08, 4.02000E-08, 2.20000E-05, 2.33000E-07, 1.12000E-08)</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="str">
         <v>Iw</v>
       </c>
-      <c r="C54" s="4" t="e">
-        <f t="array" aca="1" ref="C54" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B54&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B54&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D54" s="2" t="e">
+      <c r="C54" s="4" t="str">
+        <f t="array" aca="1" ref="C54" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B54&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B54&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">0.00000E+00, 0.00000E+00, 2.39000E-06, 0.00000E+00, 1.15000E-05, 1.34000E-05, 7.31000E-06, 0.00000E+00, 1.65000E-07, 2.86000E-06, 0.00000E+00, 1.13000E-04, 6.80000E-09, 2.94000E-05, 6.30000E-07, 0.00000E+00, 4.15000E-07, 0.00000E+00, 5.82000E-08, 7.10000E-06, 1.98000E-06, 0.00000E+00, 0.00000E+00, 3.67000E-08, 6.03000E-07, 0.00000E+00, 0.00000E+00, 4.59000E-09, 1.06000E-08, 5.57000E-07, 1.56000E-06, 5.72000E-06, 0.00000E+00, 1.62000E-05, 3.45000E-06, 0.00000E+00, 1.04000E-08, 0.00000E+00, 0.00000E+00, 6.28000E-06, 0.00000E+00, 0.00000E+00, 1.14000E-09, 2.80000E-04, 1.97000E-07, 0.00000E+00, </v>
+      </c>
+      <c r="D54" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>#REF!</v>
+        <v>Iw = (0.00000E+00, 0.00000E+00, 2.39000E-06, 0.00000E+00, 1.15000E-05, 1.34000E-05, 7.31000E-06, 0.00000E+00, 1.65000E-07, 2.86000E-06, 0.00000E+00, 1.13000E-04, 6.80000E-09, 2.94000E-05, 6.30000E-07, 0.00000E+00, 4.15000E-07, 0.00000E+00, 5.82000E-08, 7.10000E-06, 1.98000E-06, 0.00000E+00, 0.00000E+00, 3.67000E-08, 6.03000E-07, 0.00000E+00, 0.00000E+00, 4.59000E-09, 1.06000E-08, 5.57000E-07, 1.56000E-06, 5.72000E-06, 0.00000E+00, 1.62000E-05, 3.45000E-06, 0.00000E+00, 1.04000E-08, 0.00000E+00, 0.00000E+00, 6.28000E-06, 0.00000E+00, 0.00000E+00, 1.14000E-09, 2.80000E-04, 1.97000E-07, 0.00000E+00)</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="str">
         <v>βx</v>
       </c>
-      <c r="C55" s="4" t="e">
-        <f t="array" aca="1" ref="C55" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B55&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B55&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D55" s="2" t="e">
+      <c r="C55" s="4" t="str">
+        <f t="array" aca="1" ref="C55" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B55&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B55&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">1.28173E-01, -1.42314E-01, 1.78449E-01, 2.45703E-01, -1.48817E-01, 1.90016E-01, -3.08997E-02, 2.27412E-01, -4.31823E-02, 2.32830E-01, 7.81551E-02, -1.81195E-01, -2.03927E-01, 6.99328E-02, -1.73018E-01, 1.61423E-01, -1.78620E-01, -1.16781E-01, 4.82682E-02, -1.22808E-01, 4.07138E-02, 6.11456E-02, 2.12952E-01, -1.25923E-01, -3.82946E-02, 1.14895E-01, -8.74274E-03, -1.73450E-01, 2.35091E-01, 1.89466E-02, 1.48394E-01, -2.44949E-01, 1.32684E-01, 8.93709E-02, 4.72989E-02, -4.30083E-02, -1.44619E-01, 4.54835E-02, -1.31337E-01, 5.14391E-02, -1.30045E-01, -8.56207E-02, -1.38838E-01, 8.20854E-02, 1.10207E-01, 1.86297E-01, </v>
+      </c>
+      <c r="D55" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>#REF!</v>
+        <v>βx = (1.28173E-01, -1.42314E-01, 1.78449E-01, 2.45703E-01, -1.48817E-01, 1.90016E-01, -3.08997E-02, 2.27412E-01, -4.31823E-02, 2.32830E-01, 7.81551E-02, -1.81195E-01, -2.03927E-01, 6.99328E-02, -1.73018E-01, 1.61423E-01, -1.78620E-01, -1.16781E-01, 4.82682E-02, -1.22808E-01, 4.07138E-02, 6.11456E-02, 2.12952E-01, -1.25923E-01, -3.82946E-02, 1.14895E-01, -8.74274E-03, -1.73450E-01, 2.35091E-01, 1.89466E-02, 1.48394E-01, -2.44949E-01, 1.32684E-01, 8.93709E-02, 4.72989E-02, -4.30083E-02, -1.44619E-01, 4.54835E-02, -1.31337E-01, 5.14391E-02, -1.30045E-01, -8.56207E-02, -1.38838E-01, 8.20854E-02, 1.10207E-01, 1.86297E-01)</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="str">
         <v>E</v>
       </c>
-      <c r="C56" s="4" t="e">
-        <f t="array" aca="1" ref="C56" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B56&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B56&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D56" s="2" t="e">
+      <c r="C56" s="4" t="str">
+        <f t="array" aca="1" ref="C56" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B56&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B56&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, </v>
+      </c>
+      <c r="D56" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>#REF!</v>
+        <v>E = (2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11, 2.00000E+11)</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="str">
         <v>G</v>
       </c>
-      <c r="C57" s="4" t="e">
-        <f t="array" aca="1" ref="C57" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B57&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B57&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D57" s="2" t="e">
+      <c r="C57" s="4" t="str">
+        <f t="array" aca="1" ref="C57" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B57&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B57&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, </v>
+      </c>
+      <c r="D57" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>#REF!</v>
+        <v>G = (8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10, 8.00000E+10)</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="str">
-        <v>Msx</v>
+        <v>A</v>
       </c>
       <c r="C58" s="4" t="str">
-        <f t="array" aca="1" ref="C58" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B58&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B58&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v xml:space="preserve">1.02080E+03, 4.65000E+04, 6.44000E+05, 5.44000E+03, 1.78920E+06, 1.91520E+06, 1.02300E+06, 1.68560E+05, 2.02560E+05, 7.50400E+05, 1.69280E+03, 5.54400E+06, 5.02400E+04, 1.87600E+06, 4.76000E+05, 6.14400E+03, 2.39040E+05, 4.70400E+02, 1.91760E+05, 1.77840E+06, 6.63000E+05, 3.70600E+04, 2.29840E+04, 1.14840E+05, 3.63800E+05, 2.37660E+04, 5.07600E+03, 4.64400E+04, 7.51400E+04, 3.32180E+05, 5.27000E+05, 9.15800E+05, 1.91520E+03, 2.55600E+06, 1.25120E+06, 1.09800E+04, 6.48000E+04, 1.59460E+05, 2.73240E+03, 1.64920E+06, 3.11760E+03, 1.54440E+04, 2.89080E+04, 1.01160E+07, 2.47860E+05, 6.62400E+03, </v>
+        <f t="array" aca="1" ref="C58" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B58&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B58&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">9.01122E+02, 2.41439E+05, 2.99704E+06, 3.36882E+03, 2.87929E+06, 8.67663E+06, 3.65764E+07, 4.95198E+05, 5.84376E+06, 2.63536E+08, 2.70362E+03, 4.94959E+07, 2.44132E+04, 1.46487E+08, 1.34694E+06, 8.83434E+03, 1.69511E+07, 9.06401E+02, 9.43097E+04, 1.09459E+08, 1.70602E+08, 4.09221E+04, 1.91000E+04, 3.61431E+05, 1.68937E+06, 3.67121E+04, 2.95778E+03, 2.15845E+06, 3.54548E+04, 2.41045E+06, 2.56444E+07, 2.39872E+08, 1.17012E+03, 9.77946E+08, 1.12206E+06, 3.42199E+04, 2.98364E+04, 1.79190E+06, 1.76192E+03, 8.88661E+06, 6.37908E+03, 1.41681E+04, 5.94176E+05, 2.39286E+07, 2.13049E+06, 9.66878E+03, </v>
       </c>
       <c r="D58" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Msx = (1.02080E+03, 4.65000E+04, 6.44000E+05, 5.44000E+03, 1.78920E+06, 1.91520E+06, 1.02300E+06, 1.68560E+05, 2.02560E+05, 7.50400E+05, 1.69280E+03, 5.54400E+06, 5.02400E+04, 1.87600E+06, 4.76000E+05, 6.14400E+03, 2.39040E+05, 4.70400E+02, 1.91760E+05, 1.77840E+06, 6.63000E+05, 3.70600E+04, 2.29840E+04, 1.14840E+05, 3.63800E+05, 2.37660E+04, 5.07600E+03, 4.64400E+04, 7.51400E+04, 3.32180E+05, 5.27000E+05, 9.15800E+05, 1.91520E+03, 2.55600E+06, 1.25120E+06, 1.09800E+04, 6.48000E+04, 1.59460E+05, 2.73240E+03, 1.64920E+06, 3.11760E+03, 1.54440E+04, 2.89080E+04, 1.01160E+07, 2.47860E+05, 6.62400E+03)</v>
+        <v>A = (9.01122E+02, 2.41439E+05, 2.99704E+06, 3.36882E+03, 2.87929E+06, 8.67663E+06, 3.65764E+07, 4.95198E+05, 5.84376E+06, 2.63536E+08, 2.70362E+03, 4.94959E+07, 2.44132E+04, 1.46487E+08, 1.34694E+06, 8.83434E+03, 1.69511E+07, 9.06401E+02, 9.43097E+04, 1.09459E+08, 1.70602E+08, 4.09221E+04, 1.91000E+04, 3.61431E+05, 1.68937E+06, 3.67121E+04, 2.95778E+03, 2.15845E+06, 3.54548E+04, 2.41045E+06, 2.56444E+07, 2.39872E+08, 1.17012E+03, 9.77946E+08, 1.12206E+06, 3.42199E+04, 2.98364E+04, 1.79190E+06, 1.76192E+03, 8.88661E+06, 6.37908E+03, 1.41681E+04, 5.94176E+05, 2.39286E+07, 2.13049E+06, 9.66878E+03)</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="str">
-        <v>Msy</v>
+        <v>B</v>
       </c>
       <c r="C59" s="4" t="str">
-        <f t="array" aca="1" ref="C59" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B59&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B59&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v xml:space="preserve">4.96000E+02, 2.16900E+04, 2.91200E+05, 1.89760E+03, 2.96800E+05, 2.64880E+05, 4.53000E+05, 7.47600E+04, 4.44800E+04, 3.38800E+05, 7.45600E+02, 7.16800E+05, 1.04000E+04, 8.31600E+05, 2.13920E+05, 2.74880E+03, 1.01760E+05, 2.05440E+02, 2.62480E+04, 8.82000E+05, 2.98520E+05, 1.68640E+04, 6.90200E+03, 2.22120E+04, 1.61160E+05, 1.05740E+04, 2.10960E+03, 1.38600E+04, 1.51300E+04, 1.52320E+05, 2.32560E+05, 4.06600E+05, 8.78400E+02, 1.15200E+06, 1.75100E+05, 4.89600E+03, 1.23840E+04, 7.27600E+04, 1.14120E+03, 1.84680E+05, 1.08720E+03, 7.20000E+03, 5.61600E+03, 1.80000E+06, 5.54200E+04, 3.13200E+03, </v>
+        <f t="array" aca="1" ref="C59" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B59&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B59&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">7.00000E+01, 1.39200E+04, 2.01600E+05, 1.56000E+03, 3.21600E+05, 2.39200E+05, 2.46400E+05, 1.80000E+05, 1.25600E+04, 3.04800E+05, 4.48000E+02, 7.96800E+05, 3.58400E+03, 5.09600E+05, 4.78400E+05, 1.60000E+03, 2.76000E+04, 1.32800E+02, 2.32000E+04, 1.32000E+06, 1.30400E+05, 1.12800E+04, 8.80000E+03, 5.39200E+03, 6.61600E+04, 8.80000E+03, 1.40800E+03, 4.39200E+03, 8.08000E+03, 4.68800E+04, 7.42400E+04, 1.26400E+05, 2.36800E+02, 1.53600E+06, 1.24800E+05, 3.35200E+03, 3.08800E+03, 8.48000E+04, 3.09600E+02, 7.36800E+04, 3.45600E+02, 2.53600E+03, 3.21600E+03, 1.76000E+06, 1.86400E+04, 8.96000E+02, </v>
       </c>
       <c r="D59" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Msy = (4.96000E+02, 2.16900E+04, 2.91200E+05, 1.89760E+03, 2.96800E+05, 2.64880E+05, 4.53000E+05, 7.47600E+04, 4.44800E+04, 3.38800E+05, 7.45600E+02, 7.16800E+05, 1.04000E+04, 8.31600E+05, 2.13920E+05, 2.74880E+03, 1.01760E+05, 2.05440E+02, 2.62480E+04, 8.82000E+05, 2.98520E+05, 1.68640E+04, 6.90200E+03, 2.22120E+04, 1.61160E+05, 1.05740E+04, 2.10960E+03, 1.38600E+04, 1.51300E+04, 1.52320E+05, 2.32560E+05, 4.06600E+05, 8.78400E+02, 1.15200E+06, 1.75100E+05, 4.89600E+03, 1.23840E+04, 7.27600E+04, 1.14120E+03, 1.84680E+05, 1.08720E+03, 7.20000E+03, 5.61600E+03, 1.80000E+06, 5.54200E+04, 3.13200E+03)</v>
+        <v>B = (7.00000E+01, 1.39200E+04, 2.01600E+05, 1.56000E+03, 3.21600E+05, 2.39200E+05, 2.46400E+05, 1.80000E+05, 1.25600E+04, 3.04800E+05, 4.48000E+02, 7.96800E+05, 3.58400E+03, 5.09600E+05, 4.78400E+05, 1.60000E+03, 2.76000E+04, 1.32800E+02, 2.32000E+04, 1.32000E+06, 1.30400E+05, 1.12800E+04, 8.80000E+03, 5.39200E+03, 6.61600E+04, 8.80000E+03, 1.40800E+03, 4.39200E+03, 8.08000E+03, 4.68800E+04, 7.42400E+04, 1.26400E+05, 2.36800E+02, 1.53600E+06, 1.24800E+05, 3.35200E+03, 3.08800E+03, 8.48000E+04, 3.09600E+02, 7.36800E+04, 3.45600E+02, 2.53600E+03, 3.21600E+03, 1.76000E+06, 1.86400E+04, 8.96000E+02)</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B60" s="2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C60" s="4" t="e">
-        <f t="array" aca="1" ref="C60" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B60&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B60&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D60" s="2" t="e">
+      <c r="B60" s="2" t="str">
+        <v>C</v>
+      </c>
+      <c r="C60" s="4" t="str">
+        <f t="array" aca="1" ref="C60" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B60&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B60&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">0.00000E+00, 0.00000E+00, 6.69432E+04, 0.00000E+00, 3.41008E+05, 1.34103E+06, 1.24941E+06, 0.00000E+00, 1.26042E+05, 6.02970E+06, 0.00000E+00, 1.63539E+07, 1.70267E+02, 8.26623E+06, 1.52896E+04, 0.00000E+00, 2.36859E+05, 0.00000E+00, 1.35862E+03, 2.71735E+06, 3.74492E+06, 0.00000E+00, 0.00000E+00, 5.20177E+03, 2.42545E+04, 0.00000E+00, 0.00000E+00, 7.68006E+03, 2.27770E+02, 3.46036E+04, 5.48769E+05, 8.02380E+06, 0.00000E+00, 3.71024E+07, 9.85014E+04, 0.00000E+00, 2.72192E+02, 0.00000E+00, 0.00000E+00, 1.33832E+06, 0.00000E+00, 0.00000E+00, 2.00997E+03, 8.03358E+06, 4.65822E+04, 0.00000E+00, </v>
+      </c>
+      <c r="D60" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>#N/A</v>
+        <v>C = (0.00000E+00, 0.00000E+00, 6.69432E+04, 0.00000E+00, 3.41008E+05, 1.34103E+06, 1.24941E+06, 0.00000E+00, 1.26042E+05, 6.02970E+06, 0.00000E+00, 1.63539E+07, 1.70267E+02, 8.26623E+06, 1.52896E+04, 0.00000E+00, 2.36859E+05, 0.00000E+00, 1.35862E+03, 2.71735E+06, 3.74492E+06, 0.00000E+00, 0.00000E+00, 5.20177E+03, 2.42545E+04, 0.00000E+00, 0.00000E+00, 7.68006E+03, 2.27770E+02, 3.46036E+04, 5.48769E+05, 8.02380E+06, 0.00000E+00, 3.71024E+07, 9.85014E+04, 0.00000E+00, 2.72192E+02, 0.00000E+00, 0.00000E+00, 1.33832E+06, 0.00000E+00, 0.00000E+00, 2.00997E+03, 8.03358E+06, 4.65822E+04, 0.00000E+00)</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B61" s="2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C61" s="4" t="e">
-        <f t="array" aca="1" ref="C61" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B61&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B61&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D61" s="2" t="e">
+      <c r="B61" s="2" t="str">
+        <v>D0</v>
+      </c>
+      <c r="C61" s="4" t="str">
+        <f t="array" aca="1" ref="C61" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B61&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B61&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, </v>
+      </c>
+      <c r="D61" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>#N/A</v>
+        <v>D0 = (0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00)</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B62" s="2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C62" s="4" t="e">
-        <f t="array" aca="1" ref="C62" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B62&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B62&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D62" s="2" t="e">
+      <c r="B62" s="2" t="str">
+        <v>D</v>
+      </c>
+      <c r="C62" s="4" t="str">
+        <f t="array" aca="1" ref="C62" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B62&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B62&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">6.40867E-02, -7.11568E-02, 8.92243E-02, 1.22852E-01, -7.44084E-02, 9.50078E-02, -1.54499E-02, 1.13706E-01, -2.15911E-02, 1.16415E-01, 3.90775E-02, -9.05974E-02, -1.01963E-01, 3.49664E-02, -8.65092E-02, 8.07115E-02, -8.93098E-02, -5.83907E-02, 2.41341E-02, -6.14039E-02, 2.03569E-02, 3.05728E-02, 1.06476E-01, -6.29614E-02, -1.91473E-02, 5.74475E-02, -4.37137E-03, -8.67249E-02, 1.17546E-01, 9.47331E-03, 7.41969E-02, -1.22475E-01, 6.63419E-02, 4.46855E-02, 2.36494E-02, -2.15041E-02, -7.23096E-02, 2.27418E-02, -6.56684E-02, 2.57195E-02, -6.50224E-02, -4.28103E-02, -6.94191E-02, 4.10427E-02, 5.51034E-02, 9.31485E-02, </v>
+      </c>
+      <c r="D62" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>#N/A</v>
+        <v>D = (6.40867E-02, -7.11568E-02, 8.92243E-02, 1.22852E-01, -7.44084E-02, 9.50078E-02, -1.54499E-02, 1.13706E-01, -2.15911E-02, 1.16415E-01, 3.90775E-02, -9.05974E-02, -1.01963E-01, 3.49664E-02, -8.65092E-02, 8.07115E-02, -8.93098E-02, -5.83907E-02, 2.41341E-02, -6.14039E-02, 2.03569E-02, 3.05728E-02, 1.06476E-01, -6.29614E-02, -1.91473E-02, 5.74475E-02, -4.37137E-03, -8.67249E-02, 1.17546E-01, 9.47331E-03, 7.41969E-02, -1.22475E-01, 6.63419E-02, 4.46855E-02, 2.36494E-02, -2.15041E-02, -7.23096E-02, 2.27418E-02, -6.56684E-02, 2.57195E-02, -6.50224E-02, -4.28103E-02, -6.94191E-02, 4.10427E-02, 5.51034E-02, 9.31485E-02)</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B63" s="2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C63" s="4" t="e">
-        <f t="array" aca="1" ref="C63" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B63&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B63&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D63" s="2" t="e">
+      <c r="B63" s="2" t="str">
+        <v>M_o0</v>
+      </c>
+      <c r="C63" s="4" t="str">
+        <f t="array" aca="1" ref="C63" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B63&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B63&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">2.51154E+02, 5.79727E+04, 8.97126E+05, 2.29246E+03, 1.38125E+06, 3.70284E+06, 7.39670E+06, 2.98556E+05, 8.99975E+05, 4.08579E+07, 1.10055E+03, 2.91357E+07, 9.57360E+03, 3.58544E+07, 8.15457E+05, 3.75965E+03, 2.11728E+06, 3.46944E+02, 4.81261E+04, 2.10220E+07, 2.57126E+07, 2.14849E+04, 1.29646E+04, 6.18783E+04, 3.90824E+05, 1.79740E+04, 2.04072E+03, 1.61422E+05, 1.71625E+04, 4.43184E+05, 3.99708E+06, 4.42155E+07, 5.26388E+02, 1.94387E+08, 5.00557E+05, 1.07100E+04, 1.00128E+04, 3.89812E+05, 7.38574E+02, 3.54230E+06, 1.48479E+03, 5.99419E+03, 5.57239E+04, 1.53084E+07, 3.72767E+05, 2.94334E+03, </v>
+      </c>
+      <c r="D63" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>#N/A</v>
+        <v>M_o0 = (2.51154E+02, 5.79727E+04, 8.97126E+05, 2.29246E+03, 1.38125E+06, 3.70284E+06, 7.39670E+06, 2.98556E+05, 8.99975E+05, 4.08579E+07, 1.10055E+03, 2.91357E+07, 9.57360E+03, 3.58544E+07, 8.15457E+05, 3.75965E+03, 2.11728E+06, 3.46944E+02, 4.81261E+04, 2.10220E+07, 2.57126E+07, 2.14849E+04, 1.29646E+04, 6.18783E+04, 3.90824E+05, 1.79740E+04, 2.04072E+03, 1.61422E+05, 1.71625E+04, 4.43184E+05, 3.99708E+06, 4.42155E+07, 5.26388E+02, 1.94387E+08, 5.00557E+05, 1.07100E+04, 1.00128E+04, 3.89812E+05, 7.38574E+02, 3.54230E+06, 1.48479E+03, 5.99419E+03, 5.57239E+04, 1.53084E+07, 3.72767E+05, 2.94334E+03)</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" s="2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C64" s="4" t="e">
-        <f t="array" aca="1" ref="C64" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B64&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B64&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D64" s="2" t="e">
+      <c r="B64" s="2" t="str">
+        <v>M_o</v>
+      </c>
+      <c r="C64" s="4" t="str">
+        <f t="array" aca="1" ref="C64" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B64&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B64&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">3.15458E+02, 4.32847E+04, 1.20354E+06, 2.74338E+03, 1.18352E+06, 4.61784E+06, 6.85316E+06, 3.60126E+05, 7.82603E+05, 8.17736E+07, 1.21126E+03, 2.49946E+07, 7.40267E+03, 4.13406E+07, 7.07217E+05, 4.53970E+03, 1.08894E+06, 2.98032E+02, 5.04559E+04, 1.53491E+07, 2.94190E+07, 2.27724E+04, 1.51568E+04, 4.31738E+04, 3.59813E+05, 2.02064E+04, 2.02784E+03, 5.99878E+04, 2.18288E+04, 4.66607E+05, 6.32959E+06, 2.37074E+07, 6.09709E+02, 2.42938E+08, 5.27796E+05, 9.99943E+03, 8.08513E+03, 4.32687E+05, 6.31879E+02, 3.77822E+06, 1.12686E+03, 5.41826E+03, 2.80816E+04, 1.63219E+07, 5.08213E+05, 3.97868E+03, </v>
+      </c>
+      <c r="D64" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>#N/A</v>
+        <v>M_o = (3.15458E+02, 4.32847E+04, 1.20354E+06, 2.74338E+03, 1.18352E+06, 4.61784E+06, 6.85316E+06, 3.60126E+05, 7.82603E+05, 8.17736E+07, 1.21126E+03, 2.49946E+07, 7.40267E+03, 4.13406E+07, 7.07217E+05, 4.53970E+03, 1.08894E+06, 2.98032E+02, 5.04559E+04, 1.53491E+07, 2.94190E+07, 2.27724E+04, 1.51568E+04, 4.31738E+04, 3.59813E+05, 2.02064E+04, 2.02784E+03, 5.99878E+04, 2.18288E+04, 4.66607E+05, 6.32959E+06, 2.37074E+07, 6.09709E+02, 2.42938E+08, 5.27796E+05, 9.99943E+03, 8.08513E+03, 4.32687E+05, 6.31879E+02, 3.77822E+06, 1.12686E+03, 5.41826E+03, 2.80816E+04, 1.63219E+07, 5.08213E+05, 3.97868E+03)</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
@@ -3998,7 +5660,7 @@
         <v>#N/A</v>
       </c>
       <c r="C65" s="4" t="e">
-        <f t="array" aca="1" ref="C65" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B65&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B65&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
+        <f t="array" aca="1" ref="C65" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B65&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B65&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D65" s="2" t="e">
@@ -4011,7 +5673,7 @@
         <v>#N/A</v>
       </c>
       <c r="C66" s="4" t="e">
-        <f t="array" aca="1" ref="C66" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B66&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B66&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
+        <f t="array" aca="1" ref="C66" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B66&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B66&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D66" s="2" t="e">
@@ -4024,7 +5686,7 @@
         <v>#N/A</v>
       </c>
       <c r="C67" s="4" t="e">
-        <f t="array" aca="1" ref="C67" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B67&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B67&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
+        <f t="array" aca="1" ref="C67" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B67&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B67&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D67" s="2" t="e">
@@ -4037,7 +5699,7 @@
         <v>#N/A</v>
       </c>
       <c r="C68" s="4" t="e">
-        <f t="array" aca="1" ref="C68" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B68&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B68&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
+        <f t="array" aca="1" ref="C68" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B68&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B68&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D68" s="2" t="e">
@@ -4050,7 +5712,7 @@
         <v>#N/A</v>
       </c>
       <c r="C69" s="4" t="e">
-        <f t="array" aca="1" ref="C69" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B69&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B69&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
+        <f t="array" aca="1" ref="C69" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B69&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B69&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D69" s="2" t="e">
@@ -4063,7 +5725,7 @@
         <v>#N/A</v>
       </c>
       <c r="C70" s="4" t="e">
-        <f t="array" aca="1" ref="C70" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B70&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B70&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
+        <f t="array" aca="1" ref="C70" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B70&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B70&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D70" s="2" t="e">
@@ -4076,7 +5738,7 @@
         <v>#N/A</v>
       </c>
       <c r="C71" s="4" t="e">
-        <f t="array" aca="1" ref="C71" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B71&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B71&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
+        <f t="array" aca="1" ref="C71" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B71&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B71&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D71" s="2" t="e">
@@ -4089,7 +5751,7 @@
         <v>#N/A</v>
       </c>
       <c r="C72" s="4" t="e">
-        <f t="array" aca="1" ref="C72" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B72&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B72&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
+        <f t="array" aca="1" ref="C72" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B72&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B72&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D72" s="2" t="e">
@@ -4102,7 +5764,7 @@
         <v>#N/A</v>
       </c>
       <c r="C73" s="4" t="e">
-        <f t="array" aca="1" ref="C73" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B73&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B73&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
+        <f t="array" aca="1" ref="C73" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B73&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B73&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D73" s="2" t="e">
@@ -4115,7 +5777,7 @@
         <v>#N/A</v>
       </c>
       <c r="C74" s="4" t="e">
-        <f t="array" aca="1" ref="C74" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B74&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B74&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
+        <f t="array" aca="1" ref="C74" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B74&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B74&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D74" s="2" t="e">
@@ -4128,7 +5790,7 @@
         <v>#N/A</v>
       </c>
       <c r="C75" s="4" t="e">
-        <f t="array" aca="1" ref="C75" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblSection["&amp;B75&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblSection["&amp;B75&amp;"]"),"0.00000E+00")&amp;", ",""))</f>
+        <f t="array" aca="1" ref="C75" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B75&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B75&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D75" s="2" t="e">

</xml_diff>

<commit_message>
Updated unit tests for AS4100_5, tidied up the AS4100_5 module style to match PEP8 more closely.
</commit_message>
<xml_diff>
--- a/AS4100 Modules/Verification/Excel/AS4100_5 Verification.xlsx
+++ b/AS4100 Modules/Verification/Excel/AS4100_5 Verification.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11892" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Section Methods" sheetId="10" r:id="rId1"/>
     <sheet name="Mo" sheetId="12" r:id="rId2"/>
+    <sheet name="alpha_m" sheetId="13" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="74">
   <si>
     <t>Section</t>
   </si>
@@ -328,42 +329,171 @@
     </r>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>D0</t>
-  </si>
-  <si>
     <t>M_o0</t>
   </si>
   <si>
     <t>M_o</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>α</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>m_max</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>max</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>α</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <t>Ms</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d0</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <r>
+      <t>α</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="##0E+00&quot; Pa&quot;"/>
     <numFmt numFmtId="165" formatCode="##0.0000E+00&quot; m³&quot;"/>
     <numFmt numFmtId="166" formatCode="##0.00000E+00&quot; Nm&quot;"/>
     <numFmt numFmtId="167" formatCode="##0.0000E+00&quot; m&quot;"/>
     <numFmt numFmtId="168" formatCode="##0.0000E+00&quot; m⁴&quot;"/>
     <numFmt numFmtId="169" formatCode="##0.0000E+00&quot; m⁶&quot;"/>
-    <numFmt numFmtId="171" formatCode="##0.00000E+00&quot; Nm²&quot;"/>
-    <numFmt numFmtId="173" formatCode="##0.00000E+00&quot; N&quot;"/>
+    <numFmt numFmtId="170" formatCode="##0.00000E+00&quot; Nm²&quot;"/>
+    <numFmt numFmtId="171" formatCode="##0.00000E+00&quot; N&quot;"/>
+    <numFmt numFmtId="173" formatCode="##0.000E+00&quot; Nm&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,6 +552,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -449,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -464,15 +601,19 @@
     <xf numFmtId="168" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="39">
     <dxf>
       <font>
         <b val="0"/>
@@ -490,7 +631,32 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="171" formatCode="##0.00000E+00&quot; Nm²&quot;"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="##0.00000E+00&quot; Nm&quot;"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -515,13 +681,204 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="##0.0000E+00&quot; m&quot;"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="173" formatCode="##0.000E+00&quot; Nm&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="173" formatCode="##0.000E+00&quot; Nm&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="173" formatCode="##0.000E+00&quot; Nm&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="173" formatCode="##0.000E+00&quot; Nm&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFDDEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -610,31 +967,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="173" formatCode="##0.00000E+00&quot; N&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -660,12 +992,62 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="##0.00000E+00&quot; Nm²&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="171" formatCode="##0.00000E+00&quot; Nm²&quot;"/>
+      <numFmt numFmtId="170" formatCode="##0.00000E+00&quot; Nm²&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="171" formatCode="##0.00000E+00&quot; N&quot;"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -716,6 +1098,31 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="##0E+00&quot; Pa&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="##0.0000E+00&quot; m&quot;"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1125,9 +1532,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="tblIntegral" pivot="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="27"/>
-      <tableStyleElement type="headerRow" dxfId="26"/>
-      <tableStyleElement type="secondRowStripe" dxfId="25"/>
+      <tableStyleElement type="wholeTable" dxfId="38"/>
+      <tableStyleElement type="headerRow" dxfId="37"/>
+      <tableStyleElement type="secondRowStripe" dxfId="36"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1148,17 +1555,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSection" displayName="tblSection" ref="B2:G48" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSection" displayName="tblSection" ref="B2:G48" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="B2:G48"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Section" dataDxfId="22"/>
-    <tableColumn id="2" name="Zex" dataDxfId="21"/>
-    <tableColumn id="3" name="Zey" dataDxfId="20"/>
-    <tableColumn id="13" name="fy" dataDxfId="19"/>
-    <tableColumn id="19" name="Msx" dataDxfId="18">
+    <tableColumn id="1" name="Section" dataDxfId="33"/>
+    <tableColumn id="2" name="Zex" dataDxfId="32"/>
+    <tableColumn id="3" name="Zey" dataDxfId="31"/>
+    <tableColumn id="13" name="fy" dataDxfId="30"/>
+    <tableColumn id="19" name="Msx" dataDxfId="29">
       <calculatedColumnFormula>tblSection[[#This Row],[Zex]]*tblSection[[#This Row],[fy]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="Msy" dataDxfId="17">
+    <tableColumn id="20" name="Msy" dataDxfId="28">
       <calculatedColumnFormula>tblSection[[#This Row],[Zey]]*tblSection[[#This Row],[fy]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1167,37 +1574,61 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblM_o" displayName="tblM_o" ref="B2:P48" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="B2:P48"/>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Section" dataDxfId="14"/>
-    <tableColumn id="2" name="le" dataDxfId="13"/>
-    <tableColumn id="3" name="Iy" dataDxfId="12"/>
-    <tableColumn id="5" name="J" dataDxfId="11"/>
-    <tableColumn id="6" name="Iw" dataDxfId="10"/>
-    <tableColumn id="7" name="βx" dataDxfId="1"/>
-    <tableColumn id="4" name="E" dataDxfId="9"/>
-    <tableColumn id="13" name="G" dataDxfId="8"/>
-    <tableColumn id="19" name="A" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblM_o" displayName="tblM_o" ref="B2:R48" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="B2:R48"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="Section" dataDxfId="25"/>
+    <tableColumn id="2" name="le" dataDxfId="24"/>
+    <tableColumn id="3" name="Iy" dataDxfId="23"/>
+    <tableColumn id="5" name="J" dataDxfId="22"/>
+    <tableColumn id="6" name="Iw" dataDxfId="21"/>
+    <tableColumn id="7" name="βx" dataDxfId="20"/>
+    <tableColumn id="4" name="E" dataDxfId="19"/>
+    <tableColumn id="13" name="G" dataDxfId="18"/>
+    <tableColumn id="19" name="a" dataDxfId="17">
       <calculatedColumnFormula>((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iy]])/(tblM_o[[#This Row],[le]]^2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="B" dataDxfId="7">
+    <tableColumn id="20" name="b" dataDxfId="16">
       <calculatedColumnFormula>tblM_o[[#This Row],[G]]*tblM_o[[#This Row],[J]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="C" dataDxfId="0">
+    <tableColumn id="9" name="c" dataDxfId="15">
       <calculatedColumnFormula>(((PI()^2*tblM_o[[#This Row],[E]]*tblM_o[[#This Row],[Iw]])/(tblM_o[[#This Row],[le]]^2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="D0" dataDxfId="6">
+    <tableColumn id="8" name="d0" dataDxfId="14">
       <calculatedColumnFormula>0</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="D" dataDxfId="4">
+    <tableColumn id="10" name="d" dataDxfId="13">
       <calculatedColumnFormula>tblM_o[[#This Row],[βx]]/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="M_o0" dataDxfId="3">
-      <calculatedColumnFormula>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</calculatedColumnFormula>
+    <tableColumn id="11" name="M_o0" dataDxfId="12">
+      <calculatedColumnFormula>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="M_o" dataDxfId="2">
-      <calculatedColumnFormula>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</calculatedColumnFormula>
+    <tableColumn id="12" name="M_o" dataDxfId="11">
+      <calculatedColumnFormula>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" name="Ms" dataDxfId="1">
+      <calculatedColumnFormula>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" name="αs" dataDxfId="0">
+      <calculatedColumnFormula>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="tblIntegral" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tblalpha_m" displayName="tblalpha_m" ref="B2:H48" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="B2:H48"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Section" dataDxfId="8"/>
+    <tableColumn id="2" name="Mmax" dataDxfId="4"/>
+    <tableColumn id="3" name="M2" dataDxfId="7"/>
+    <tableColumn id="5" name="M3" dataDxfId="6"/>
+    <tableColumn id="6" name="M4" dataDxfId="5"/>
+    <tableColumn id="7" name="αm_max" dataDxfId="3"/>
+    <tableColumn id="19" name="αm" dataDxfId="2">
+      <calculatedColumnFormula>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="tblIntegral" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1503,24 +1934,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G75"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="14.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="14.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.7109375" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="2:7" ht="11.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2902,33 +3333,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P75"/>
+  <dimension ref="B1:R75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="2" customWidth="1"/>
-    <col min="3" max="7" width="14.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="2" customWidth="1"/>
-    <col min="10" max="11" width="16.6640625" style="2" customWidth="1"/>
-    <col min="12" max="13" width="15.44140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="3.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="2" customWidth="1"/>
+    <col min="3" max="7" width="14.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="2" customWidth="1"/>
+    <col min="10" max="11" width="16.7109375" style="2" customWidth="1"/>
+    <col min="12" max="13" width="15.42578125" style="2" customWidth="1"/>
+    <col min="14" max="17" width="15.28515625" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.2">
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="2:16" ht="11.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2954,28 +3384,34 @@
         <v>55</v>
       </c>
       <c r="J2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="P2" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q2" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>40</v>
       </c>
@@ -3021,15 +3457,23 @@
         <v>6.408672244422825E-2</v>
       </c>
       <c r="O3" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>251.15440985825023</v>
       </c>
       <c r="P3" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>315.45830530974268</v>
       </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q3" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>1020.8</v>
+      </c>
+      <c r="R3" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.26063373841994347</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>49</v>
       </c>
@@ -3075,15 +3519,23 @@
         <v>-7.1156789108930668E-2</v>
       </c>
       <c r="O4" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>57972.693837691761</v>
       </c>
       <c r="P4" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>43284.721221093743</v>
       </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q4" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>46500</v>
+      </c>
+      <c r="R4" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.57832466440965946</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
@@ -3129,15 +3581,23 @@
         <v>8.9224281472892242E-2</v>
       </c>
       <c r="O5" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>897125.67581513233</v>
       </c>
       <c r="P5" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>1203539.9843339205</v>
       </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q5" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>644000</v>
+      </c>
+      <c r="R5" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.76663959673217619</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
@@ -3183,15 +3643,23 @@
         <v>0.12285168961061749</v>
       </c>
       <c r="O6" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>2292.4561770473465</v>
       </c>
       <c r="P6" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>2743.3797871244597</v>
       </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q6" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>5440</v>
+      </c>
+      <c r="R6" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.3899610168342858</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -3237,15 +3705,23 @@
         <v>-7.4408359044419919E-2</v>
       </c>
       <c r="O7" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>1381246.8155025893</v>
       </c>
       <c r="P7" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>1183520.0882903179</v>
       </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q7" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>1789200</v>
+      </c>
+      <c r="R7" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.47234596704919546</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -3291,15 +3767,23 @@
         <v>9.500778019081707E-2</v>
       </c>
       <c r="O8" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>3702841.0727126608</v>
       </c>
       <c r="P8" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>4617839.5004720306</v>
       </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q8" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>1915200</v>
+      </c>
+      <c r="R8" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.81976440493548342</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
@@ -3345,15 +3829,23 @@
         <v>-1.5449874826186205E-2</v>
       </c>
       <c r="O9" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>7396703.8850564715</v>
       </c>
       <c r="P9" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>6853158.6231102394</v>
       </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q9" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>1023000</v>
+      </c>
+      <c r="R9" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.95351829789990084</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
@@ -3399,15 +3891,23 @@
         <v>0.1137062230075499</v>
       </c>
       <c r="O10" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>298555.8082890205</v>
       </c>
       <c r="P10" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>360126.16533973371</v>
       </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q10" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>168560</v>
+      </c>
+      <c r="R10" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.79567251834421415</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
@@ -3453,15 +3953,23 @@
         <v>-2.1591127876856964E-2</v>
       </c>
       <c r="O11" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>899975.17182241625</v>
       </c>
       <c r="P11" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>782603.35481326585</v>
       </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q11" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>202560</v>
+      </c>
+      <c r="R11" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.89547274218542217</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -3507,15 +4015,23 @@
         <v>0.11641512012611857</v>
       </c>
       <c r="O12" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>40857879.141069613</v>
       </c>
       <c r="P12" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>81773579.312149212</v>
       </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q12" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>750400</v>
+      </c>
+      <c r="R12" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>1.0337391350551755</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
@@ -3561,15 +4077,23 @@
         <v>3.9077536319290729E-2</v>
       </c>
       <c r="O13" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>1100.5544578991326</v>
       </c>
       <c r="P13" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>1211.2646023190814</v>
       </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q13" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>1692.8</v>
+      </c>
+      <c r="R13" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.49681039149822526</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
@@ -3615,15 +4139,23 @@
         <v>-9.0597376713119404E-2</v>
       </c>
       <c r="O14" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>29135719.663914114</v>
       </c>
       <c r="P14" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>24994575.752043754</v>
       </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q14" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>5544000</v>
+      </c>
+      <c r="R14" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.914632445270818</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
@@ -3669,15 +4201,23 @@
         <v>-0.10196337546948836</v>
       </c>
       <c r="O15" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>9573.6011213133443</v>
       </c>
       <c r="P15" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>7402.6709695861746</v>
       </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q15" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>50240</v>
+      </c>
+      <c r="R15" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.13051978953796475</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
@@ -3723,15 +4263,23 @@
         <v>3.4966387529702853E-2</v>
       </c>
       <c r="O16" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>35854440.741187237</v>
       </c>
       <c r="P16" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>41340566.53916686</v>
       </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q16" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>1876000</v>
+      </c>
+      <c r="R16" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>1.0123596056561877</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
@@ -3777,15 +4325,23 @@
         <v>-8.6509173118239413E-2</v>
       </c>
       <c r="O17" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>815456.56793715735</v>
       </c>
       <c r="P17" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>707217.0675270377</v>
       </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q17" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>476000</v>
+      </c>
+      <c r="R17" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.71110029194383695</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>44</v>
       </c>
@@ -3831,15 +4387,23 @@
         <v>8.0711474193731064E-2</v>
       </c>
       <c r="O18" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>3759.6477050730509</v>
       </c>
       <c r="P18" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>4539.698190885847</v>
       </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q18" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>6144</v>
+      </c>
+      <c r="R18" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.5068279426169684</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
@@ -3885,15 +4449,23 @@
         <v>-8.9309811629107672E-2</v>
       </c>
       <c r="O19" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>2117276.1470823628</v>
       </c>
       <c r="P19" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>1088936.1665291372</v>
       </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q19" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>239040.00000000003</v>
+      </c>
+      <c r="R19" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.91583339205540537</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
@@ -3939,15 +4511,23 @@
         <v>-5.8390742810850577E-2</v>
       </c>
       <c r="O20" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>346.94380709787896</v>
       </c>
       <c r="P20" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>298.03200369196639</v>
       </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q20" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>470.4</v>
+      </c>
+      <c r="R20" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.45898635365555679</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>38</v>
       </c>
@@ -3993,15 +4573,23 @@
         <v>2.4134111206316616E-2</v>
       </c>
       <c r="O21" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>48126.05278538631</v>
       </c>
       <c r="P21" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>50455.92701998767</v>
       </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q21" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>191760.00000000003</v>
+      </c>
+      <c r="R21" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.22564413719694548</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
@@ -4047,15 +4635,23 @@
         <v>-6.1403914150175182E-2</v>
       </c>
       <c r="O22" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>21022037.475277971</v>
       </c>
       <c r="P22" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>15349128.850817373</v>
       </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q22" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>1778400</v>
+      </c>
+      <c r="R22" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.97203509321246184</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
@@ -4101,15 +4697,23 @@
         <v>2.0356878038573195E-2</v>
       </c>
       <c r="O23" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>25712586.527343422</v>
       </c>
       <c r="P23" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>29418987.744043078</v>
       </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q23" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>663000</v>
+      </c>
+      <c r="R23" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>1.0257965710883561</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>48</v>
       </c>
@@ -4155,15 +4759,23 @@
         <v>3.0572802025874091E-2</v>
       </c>
       <c r="O24" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>21484.898194581579</v>
       </c>
       <c r="P24" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>22772.396340699379</v>
       </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q24" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>37060</v>
+      </c>
+      <c r="R24" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.4495439703943645</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>34</v>
       </c>
@@ -4209,15 +4821,23 @@
         <v>0.10647596416257829</v>
       </c>
       <c r="O25" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>12964.560698374424</v>
       </c>
       <c r="P25" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>15156.78780585297</v>
       </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q25" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>22984</v>
+      </c>
+      <c r="R25" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.47139119293605014</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
@@ -4263,15 +4883,23 @@
         <v>-6.296137278731373E-2</v>
       </c>
       <c r="O26" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>61878.262672481171</v>
       </c>
       <c r="P26" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>43173.793697935238</v>
       </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q26" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>114840</v>
+      </c>
+      <c r="R26" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.30853029602352799</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
@@ -4317,15 +4945,23 @@
         <v>-1.9147316996619007E-2</v>
       </c>
       <c r="O27" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>390823.66102751798</v>
       </c>
       <c r="P27" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>359813.15466422978</v>
       </c>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q27" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>363800</v>
+      </c>
+      <c r="R27" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.59668967741886203</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>47</v>
       </c>
@@ -4371,15 +5007,23 @@
         <v>5.7447527717466113E-2</v>
       </c>
       <c r="O28" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>17974.039008309312</v>
       </c>
       <c r="P28" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>20206.365459672474</v>
       </c>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q28" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>23766</v>
+      </c>
+      <c r="R28" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.55049036745774627</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>32</v>
       </c>
@@ -4425,15 +5069,23 @@
         <v>-4.3713678957016389E-3</v>
       </c>
       <c r="O29" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>2040.7235856045675</v>
       </c>
       <c r="P29" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>2027.8350045230263</v>
       </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q29" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>5076</v>
+      </c>
+      <c r="R29" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.32449134252617423</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>36</v>
       </c>
@@ -4479,15 +5131,23 @@
         <v>-8.6724896465800644E-2</v>
       </c>
       <c r="O30" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>161421.56849223017</v>
       </c>
       <c r="P30" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>59987.813901311281</v>
       </c>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q30" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>46440</v>
+      </c>
+      <c r="R30" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.67381800398960301</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>37</v>
       </c>
@@ -4533,15 +5193,23 @@
         <v>0.11754566123706481</v>
       </c>
       <c r="O31" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>17162.468885165119</v>
       </c>
       <c r="P31" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>21828.783262169007</v>
       </c>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q31" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>75140</v>
+      </c>
+      <c r="R31" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.24672101418485476</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
@@ -4587,15 +5255,23 @@
         <v>9.4733095406588641E-3</v>
       </c>
       <c r="O32" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>443183.83589399373</v>
       </c>
       <c r="P32" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>466606.64226913889</v>
       </c>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q32" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>332180</v>
+      </c>
+      <c r="R32" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.69644519368783386</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>18</v>
       </c>
@@ -4641,15 +5317,23 @@
         <v>7.4196854049522143E-2</v>
       </c>
       <c r="O33" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>3997083.2947414783</v>
       </c>
       <c r="P33" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>6329590.0202653678</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q33" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>527000</v>
+      </c>
+      <c r="R33" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.99047463901726251</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>8</v>
       </c>
@@ -4695,15 +5379,23 @@
         <v>-0.12247455366494103</v>
       </c>
       <c r="O34" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>44215478.896987282</v>
       </c>
       <c r="P34" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>23707429.814660929</v>
       </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q34" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>915799.99999999988</v>
+      </c>
+      <c r="R34" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>1.0163113680836839</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>41</v>
       </c>
@@ -4749,15 +5441,23 @@
         <v>6.6341914517829725E-2</v>
       </c>
       <c r="O35" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>526.38822427003595</v>
       </c>
       <c r="P35" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>609.70949786764584</v>
       </c>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q35" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>1915.2</v>
+      </c>
+      <c r="R35" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.26752992335754328</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>12</v>
       </c>
@@ -4803,15 +5503,23 @@
         <v>4.468546073276855E-2</v>
       </c>
       <c r="O36" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>194386866.50937274</v>
       </c>
       <c r="P36" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>242938358.75441101</v>
       </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q36" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>2556000</v>
+      </c>
+      <c r="R36" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>1.0329369449252437</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>2</v>
       </c>
@@ -4857,15 +5565,23 @@
         <v>2.3649426468545315E-2</v>
       </c>
       <c r="O37" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>500557.23170788836</v>
       </c>
       <c r="P37" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>527796.18664483225</v>
       </c>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q37" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>1251200</v>
+      </c>
+      <c r="R37" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.33920267692426964</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>45</v>
       </c>
@@ -4911,15 +5627,23 @@
         <v>-2.1504133336327613E-2</v>
       </c>
       <c r="O38" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>10710.047946741732</v>
       </c>
       <c r="P38" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>9999.4289236204531</v>
       </c>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q38" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>10980</v>
+      </c>
+      <c r="R38" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.57163668050326255</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>26</v>
       </c>
@@ -4965,15 +5689,23 @@
         <v>-7.2309588477194459E-2</v>
       </c>
       <c r="O39" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>10012.790344830153</v>
       </c>
       <c r="P39" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>8085.1303422081046</v>
       </c>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q39" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>64800.000000000007</v>
+      </c>
+      <c r="R39" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.11101211587802169</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>50</v>
       </c>
@@ -5019,15 +5751,23 @@
         <v>2.2741772126096821E-2</v>
       </c>
       <c r="O40" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>389811.75196021254</v>
       </c>
       <c r="P40" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>432687.02661249664</v>
       </c>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q40" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>159460</v>
+      </c>
+      <c r="R40" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.84137381308386294</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>30</v>
       </c>
@@ -5073,15 +5813,23 @@
         <v>-6.5668368949401951E-2</v>
       </c>
       <c r="O41" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>738.57377456446557</v>
       </c>
       <c r="P41" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>631.87905946789692</v>
       </c>
-    </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q41" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>2732.4</v>
+      </c>
+      <c r="R41" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.20039022349283009</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>13</v>
       </c>
@@ -5127,15 +5875,23 @@
         <v>2.5719536120148767E-2</v>
       </c>
       <c r="O42" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>3542298.2574965428</v>
       </c>
       <c r="P42" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>3778223.6578902965</v>
       </c>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q42" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>1649200</v>
+      </c>
+      <c r="R42" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.80982301829286463</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>31</v>
       </c>
@@ -5181,15 +5937,23 @@
         <v>-6.5022369406948721E-2</v>
       </c>
       <c r="O43" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>1484.7934747110385</v>
       </c>
       <c r="P43" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>1126.8577327535636</v>
       </c>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q43" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>3117.6</v>
+      </c>
+      <c r="R43" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.29847201336402468</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>46</v>
       </c>
@@ -5235,15 +5999,23 @@
         <v>-4.281034868755787E-2</v>
       </c>
       <c r="O44" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>5994.1881794550982</v>
       </c>
       <c r="P44" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>5418.2562928410998</v>
       </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q44" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>15444</v>
+      </c>
+      <c r="R44" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.29099302021774109</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>35</v>
       </c>
@@ -5289,15 +6061,23 @@
         <v>-6.9419100182676635E-2</v>
       </c>
       <c r="O45" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>55723.862156633331</v>
       </c>
       <c r="P45" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>28081.593111355083</v>
       </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q45" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>28908</v>
+      </c>
+      <c r="R45" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.59126808295294964</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>1</v>
       </c>
@@ -5343,15 +6123,23 @@
         <v>4.1042716149252173E-2</v>
       </c>
       <c r="O46" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>15308383.093127273</v>
       </c>
       <c r="P46" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>16321947.83875609</v>
       </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q46" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>10116000</v>
+      </c>
+      <c r="R46" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.73189226161188159</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>29</v>
       </c>
@@ -5397,15 +6185,23 @@
         <v>5.5103382622603447E-2</v>
       </c>
       <c r="O47" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>372766.78983140807</v>
       </c>
       <c r="P47" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>508213.01026589843</v>
       </c>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q47" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>247860.00000000003</v>
+      </c>
+      <c r="R47" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.78701793666730535</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>43</v>
       </c>
@@ -5451,12 +6247,20 @@
         <v>9.3148487822567627E-2</v>
       </c>
       <c r="O48" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D0]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D0]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d0]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d0]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>2943.3359654028018</v>
       </c>
       <c r="P48" s="17">
-        <f>SQRT(tblM_o[[#This Row],[A]])*(SQRT(tblM_o[[#This Row],[B]]+tblM_o[[#This Row],[C]]+(tblM_o[[#This Row],[D]]^2)*tblM_o[[#This Row],[A]])+tblM_o[[#This Row],[D]]*SQRT(tblM_o[[#This Row],[A]]))</f>
+        <f>SQRT(tblM_o[[#This Row],[a]])*(SQRT(tblM_o[[#This Row],[b]]+tblM_o[[#This Row],[c]]+(tblM_o[[#This Row],[d]]^2)*tblM_o[[#This Row],[a]])+tblM_o[[#This Row],[d]]*SQRT(tblM_o[[#This Row],[a]]))</f>
         <v>3978.6778502111547</v>
+      </c>
+      <c r="Q48" s="17">
+        <f>INDEX(tblSection[Msx],MATCH(tblM_o[[#This Row],[Section]],tblSection[Section],0))</f>
+        <v>6624</v>
+      </c>
+      <c r="R48" s="21">
+        <f>0.6*(SQRT((tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]])^2+3)-(tblM_o[[#This Row],[Ms]]/tblM_o[[#This Row],[M_o]]))</f>
+        <v>0.44255039946355762</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
@@ -5566,7 +6370,7 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="str">
-        <v>A</v>
+        <v>a</v>
       </c>
       <c r="C58" s="4" t="str">
         <f t="array" aca="1" ref="C58" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B58&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B58&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
@@ -5574,12 +6378,12 @@
       </c>
       <c r="D58" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>A = (9.01122E+02, 2.41439E+05, 2.99704E+06, 3.36882E+03, 2.87929E+06, 8.67663E+06, 3.65764E+07, 4.95198E+05, 5.84376E+06, 2.63536E+08, 2.70362E+03, 4.94959E+07, 2.44132E+04, 1.46487E+08, 1.34694E+06, 8.83434E+03, 1.69511E+07, 9.06401E+02, 9.43097E+04, 1.09459E+08, 1.70602E+08, 4.09221E+04, 1.91000E+04, 3.61431E+05, 1.68937E+06, 3.67121E+04, 2.95778E+03, 2.15845E+06, 3.54548E+04, 2.41045E+06, 2.56444E+07, 2.39872E+08, 1.17012E+03, 9.77946E+08, 1.12206E+06, 3.42199E+04, 2.98364E+04, 1.79190E+06, 1.76192E+03, 8.88661E+06, 6.37908E+03, 1.41681E+04, 5.94176E+05, 2.39286E+07, 2.13049E+06, 9.66878E+03)</v>
+        <v>a = (9.01122E+02, 2.41439E+05, 2.99704E+06, 3.36882E+03, 2.87929E+06, 8.67663E+06, 3.65764E+07, 4.95198E+05, 5.84376E+06, 2.63536E+08, 2.70362E+03, 4.94959E+07, 2.44132E+04, 1.46487E+08, 1.34694E+06, 8.83434E+03, 1.69511E+07, 9.06401E+02, 9.43097E+04, 1.09459E+08, 1.70602E+08, 4.09221E+04, 1.91000E+04, 3.61431E+05, 1.68937E+06, 3.67121E+04, 2.95778E+03, 2.15845E+06, 3.54548E+04, 2.41045E+06, 2.56444E+07, 2.39872E+08, 1.17012E+03, 9.77946E+08, 1.12206E+06, 3.42199E+04, 2.98364E+04, 1.79190E+06, 1.76192E+03, 8.88661E+06, 6.37908E+03, 1.41681E+04, 5.94176E+05, 2.39286E+07, 2.13049E+06, 9.66878E+03)</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="str">
-        <v>B</v>
+        <v>b</v>
       </c>
       <c r="C59" s="4" t="str">
         <f t="array" aca="1" ref="C59" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B59&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B59&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
@@ -5587,12 +6391,12 @@
       </c>
       <c r="D59" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>B = (7.00000E+01, 1.39200E+04, 2.01600E+05, 1.56000E+03, 3.21600E+05, 2.39200E+05, 2.46400E+05, 1.80000E+05, 1.25600E+04, 3.04800E+05, 4.48000E+02, 7.96800E+05, 3.58400E+03, 5.09600E+05, 4.78400E+05, 1.60000E+03, 2.76000E+04, 1.32800E+02, 2.32000E+04, 1.32000E+06, 1.30400E+05, 1.12800E+04, 8.80000E+03, 5.39200E+03, 6.61600E+04, 8.80000E+03, 1.40800E+03, 4.39200E+03, 8.08000E+03, 4.68800E+04, 7.42400E+04, 1.26400E+05, 2.36800E+02, 1.53600E+06, 1.24800E+05, 3.35200E+03, 3.08800E+03, 8.48000E+04, 3.09600E+02, 7.36800E+04, 3.45600E+02, 2.53600E+03, 3.21600E+03, 1.76000E+06, 1.86400E+04, 8.96000E+02)</v>
+        <v>b = (7.00000E+01, 1.39200E+04, 2.01600E+05, 1.56000E+03, 3.21600E+05, 2.39200E+05, 2.46400E+05, 1.80000E+05, 1.25600E+04, 3.04800E+05, 4.48000E+02, 7.96800E+05, 3.58400E+03, 5.09600E+05, 4.78400E+05, 1.60000E+03, 2.76000E+04, 1.32800E+02, 2.32000E+04, 1.32000E+06, 1.30400E+05, 1.12800E+04, 8.80000E+03, 5.39200E+03, 6.61600E+04, 8.80000E+03, 1.40800E+03, 4.39200E+03, 8.08000E+03, 4.68800E+04, 7.42400E+04, 1.26400E+05, 2.36800E+02, 1.53600E+06, 1.24800E+05, 3.35200E+03, 3.08800E+03, 8.48000E+04, 3.09600E+02, 7.36800E+04, 3.45600E+02, 2.53600E+03, 3.21600E+03, 1.76000E+06, 1.86400E+04, 8.96000E+02)</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="str">
-        <v>C</v>
+        <v>c</v>
       </c>
       <c r="C60" s="4" t="str">
         <f t="array" aca="1" ref="C60" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B60&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B60&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
@@ -5600,12 +6404,12 @@
       </c>
       <c r="D60" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>C = (0.00000E+00, 0.00000E+00, 6.69432E+04, 0.00000E+00, 3.41008E+05, 1.34103E+06, 1.24941E+06, 0.00000E+00, 1.26042E+05, 6.02970E+06, 0.00000E+00, 1.63539E+07, 1.70267E+02, 8.26623E+06, 1.52896E+04, 0.00000E+00, 2.36859E+05, 0.00000E+00, 1.35862E+03, 2.71735E+06, 3.74492E+06, 0.00000E+00, 0.00000E+00, 5.20177E+03, 2.42545E+04, 0.00000E+00, 0.00000E+00, 7.68006E+03, 2.27770E+02, 3.46036E+04, 5.48769E+05, 8.02380E+06, 0.00000E+00, 3.71024E+07, 9.85014E+04, 0.00000E+00, 2.72192E+02, 0.00000E+00, 0.00000E+00, 1.33832E+06, 0.00000E+00, 0.00000E+00, 2.00997E+03, 8.03358E+06, 4.65822E+04, 0.00000E+00)</v>
+        <v>c = (0.00000E+00, 0.00000E+00, 6.69432E+04, 0.00000E+00, 3.41008E+05, 1.34103E+06, 1.24941E+06, 0.00000E+00, 1.26042E+05, 6.02970E+06, 0.00000E+00, 1.63539E+07, 1.70267E+02, 8.26623E+06, 1.52896E+04, 0.00000E+00, 2.36859E+05, 0.00000E+00, 1.35862E+03, 2.71735E+06, 3.74492E+06, 0.00000E+00, 0.00000E+00, 5.20177E+03, 2.42545E+04, 0.00000E+00, 0.00000E+00, 7.68006E+03, 2.27770E+02, 3.46036E+04, 5.48769E+05, 8.02380E+06, 0.00000E+00, 3.71024E+07, 9.85014E+04, 0.00000E+00, 2.72192E+02, 0.00000E+00, 0.00000E+00, 1.33832E+06, 0.00000E+00, 0.00000E+00, 2.00997E+03, 8.03358E+06, 4.65822E+04, 0.00000E+00)</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="str">
-        <v>D0</v>
+        <v>d0</v>
       </c>
       <c r="C61" s="4" t="str">
         <f t="array" aca="1" ref="C61" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B61&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B61&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
@@ -5613,12 +6417,12 @@
       </c>
       <c r="D61" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>D0 = (0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00)</v>
+        <v>d0 = (0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00, 0.00000E+00)</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="str">
-        <v>D</v>
+        <v>d</v>
       </c>
       <c r="C62" s="4" t="str">
         <f t="array" aca="1" ref="C62" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B62&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B62&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
@@ -5626,7 +6430,7 @@
       </c>
       <c r="D62" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>D = (6.40867E-02, -7.11568E-02, 8.92243E-02, 1.22852E-01, -7.44084E-02, 9.50078E-02, -1.54499E-02, 1.13706E-01, -2.15911E-02, 1.16415E-01, 3.90775E-02, -9.05974E-02, -1.01963E-01, 3.49664E-02, -8.65092E-02, 8.07115E-02, -8.93098E-02, -5.83907E-02, 2.41341E-02, -6.14039E-02, 2.03569E-02, 3.05728E-02, 1.06476E-01, -6.29614E-02, -1.91473E-02, 5.74475E-02, -4.37137E-03, -8.67249E-02, 1.17546E-01, 9.47331E-03, 7.41969E-02, -1.22475E-01, 6.63419E-02, 4.46855E-02, 2.36494E-02, -2.15041E-02, -7.23096E-02, 2.27418E-02, -6.56684E-02, 2.57195E-02, -6.50224E-02, -4.28103E-02, -6.94191E-02, 4.10427E-02, 5.51034E-02, 9.31485E-02)</v>
+        <v>d = (6.40867E-02, -7.11568E-02, 8.92243E-02, 1.22852E-01, -7.44084E-02, 9.50078E-02, -1.54499E-02, 1.13706E-01, -2.15911E-02, 1.16415E-01, 3.90775E-02, -9.05974E-02, -1.01963E-01, 3.49664E-02, -8.65092E-02, 8.07115E-02, -8.93098E-02, -5.83907E-02, 2.41341E-02, -6.14039E-02, 2.03569E-02, 3.05728E-02, 1.06476E-01, -6.29614E-02, -1.91473E-02, 5.74475E-02, -4.37137E-03, -8.67249E-02, 1.17546E-01, 9.47331E-03, 7.41969E-02, -1.22475E-01, 6.63419E-02, 4.46855E-02, 2.36494E-02, -2.15041E-02, -7.23096E-02, 2.27418E-02, -6.56684E-02, 2.57195E-02, -6.50224E-02, -4.28103E-02, -6.94191E-02, 4.10427E-02, 5.51034E-02, 9.31485E-02)</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
@@ -5656,11 +6460,1509 @@
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65" s="2" t="str">
+        <v>Ms</v>
+      </c>
+      <c r="C65" s="4" t="str">
+        <f t="array" aca="1" ref="C65" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B65&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B65&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">1.02080E+03, 4.65000E+04, 6.44000E+05, 5.44000E+03, 1.78920E+06, 1.91520E+06, 1.02300E+06, 1.68560E+05, 2.02560E+05, 7.50400E+05, 1.69280E+03, 5.54400E+06, 5.02400E+04, 1.87600E+06, 4.76000E+05, 6.14400E+03, 2.39040E+05, 4.70400E+02, 1.91760E+05, 1.77840E+06, 6.63000E+05, 3.70600E+04, 2.29840E+04, 1.14840E+05, 3.63800E+05, 2.37660E+04, 5.07600E+03, 4.64400E+04, 7.51400E+04, 3.32180E+05, 5.27000E+05, 9.15800E+05, 1.91520E+03, 2.55600E+06, 1.25120E+06, 1.09800E+04, 6.48000E+04, 1.59460E+05, 2.73240E+03, 1.64920E+06, 3.11760E+03, 1.54440E+04, 2.89080E+04, 1.01160E+07, 2.47860E+05, 6.62400E+03, </v>
+      </c>
+      <c r="D65" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Ms = (1.02080E+03, 4.65000E+04, 6.44000E+05, 5.44000E+03, 1.78920E+06, 1.91520E+06, 1.02300E+06, 1.68560E+05, 2.02560E+05, 7.50400E+05, 1.69280E+03, 5.54400E+06, 5.02400E+04, 1.87600E+06, 4.76000E+05, 6.14400E+03, 2.39040E+05, 4.70400E+02, 1.91760E+05, 1.77840E+06, 6.63000E+05, 3.70600E+04, 2.29840E+04, 1.14840E+05, 3.63800E+05, 2.37660E+04, 5.07600E+03, 4.64400E+04, 7.51400E+04, 3.32180E+05, 5.27000E+05, 9.15800E+05, 1.91520E+03, 2.55600E+06, 1.25120E+06, 1.09800E+04, 6.48000E+04, 1.59460E+05, 2.73240E+03, 1.64920E+06, 3.11760E+03, 1.54440E+04, 2.89080E+04, 1.01160E+07, 2.47860E+05, 6.62400E+03)</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" s="2" t="str">
+        <v>αs</v>
+      </c>
+      <c r="C66" s="4" t="str">
+        <f t="array" aca="1" ref="C66" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B66&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B66&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">2.60634E-01, 5.78325E-01, 7.66640E-01, 3.89961E-01, 4.72346E-01, 8.19764E-01, 9.53518E-01, 7.95673E-01, 8.95473E-01, 1.03374E+00, 4.96810E-01, 9.14632E-01, 1.30520E-01, 1.01236E+00, 7.11100E-01, 5.06828E-01, 9.15833E-01, 4.58986E-01, 2.25644E-01, 9.72035E-01, 1.02580E+00, 4.49544E-01, 4.71391E-01, 3.08530E-01, 5.96690E-01, 5.50490E-01, 3.24491E-01, 6.73818E-01, 2.46721E-01, 6.96445E-01, 9.90475E-01, 1.01631E+00, 2.67530E-01, 1.03294E+00, 3.39203E-01, 5.71637E-01, 1.11012E-01, 8.41374E-01, 2.00390E-01, 8.09823E-01, 2.98472E-01, 2.90993E-01, 5.91268E-01, 7.31892E-01, 7.87018E-01, 4.42550E-01, </v>
+      </c>
+      <c r="D66" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>αs = (2.60634E-01, 5.78325E-01, 7.66640E-01, 3.89961E-01, 4.72346E-01, 8.19764E-01, 9.53518E-01, 7.95673E-01, 8.95473E-01, 1.03374E+00, 4.96810E-01, 9.14632E-01, 1.30520E-01, 1.01236E+00, 7.11100E-01, 5.06828E-01, 9.15833E-01, 4.58986E-01, 2.25644E-01, 9.72035E-01, 1.02580E+00, 4.49544E-01, 4.71391E-01, 3.08530E-01, 5.96690E-01, 5.50490E-01, 3.24491E-01, 6.73818E-01, 2.46721E-01, 6.96445E-01, 9.90475E-01, 1.01631E+00, 2.67530E-01, 1.03294E+00, 3.39203E-01, 5.71637E-01, 1.11012E-01, 8.41374E-01, 2.00390E-01, 8.09823E-01, 2.98472E-01, 2.90993E-01, 5.91268E-01, 7.31892E-01, 7.87018E-01, 4.42550E-01)</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C67" s="4" t="e">
+        <f t="array" aca="1" ref="C67" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B67&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B67&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D67" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B68" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C68" s="4" t="e">
+        <f t="array" aca="1" ref="C68" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B68&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B68&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D68" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B69" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C69" s="4" t="e">
+        <f t="array" aca="1" ref="C69" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B69&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B69&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D69" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B70" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C70" s="4" t="e">
+        <f t="array" aca="1" ref="C70" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B70&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B70&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D70" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B71" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C71" s="4" t="e">
+        <f t="array" aca="1" ref="C71" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B71&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B71&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D71" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B72" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C72" s="4" t="e">
+        <f t="array" aca="1" ref="C72" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B72&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B72&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D72" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B73" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C73" s="4" t="e">
+        <f t="array" aca="1" ref="C73" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B73&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B73&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D73" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B74" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C74" s="4" t="e">
+        <f t="array" aca="1" ref="C74" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B74&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B74&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D74" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B75" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C75" s="4" t="e">
+        <f t="array" aca="1" ref="C75" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B75&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B75&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D75" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H75"/>
+  <sheetViews>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="2" customWidth="1"/>
+    <col min="3" max="7" width="14.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="2:8" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="19">
+        <v>467469.33178514382</v>
+      </c>
+      <c r="D3" s="19">
+        <v>-467469.33178514382</v>
+      </c>
+      <c r="E3" s="19">
+        <v>309832.21790736692</v>
+      </c>
+      <c r="F3" s="19">
+        <v>-367539.91585863155</v>
+      </c>
+      <c r="G3" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H3" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.185180414451122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="19">
+        <v>349510.14228425699</v>
+      </c>
+      <c r="D4" s="19">
+        <v>-142941.45165516349</v>
+      </c>
+      <c r="E4" s="19">
+        <v>349510.14228425699</v>
+      </c>
+      <c r="F4" s="19">
+        <v>-272333.14025197655</v>
+      </c>
+      <c r="G4" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H4" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.2762160577217003</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="19">
+        <v>347664.29452958249</v>
+      </c>
+      <c r="D5" s="19">
+        <v>33789.301898081438</v>
+      </c>
+      <c r="E5" s="19">
+        <v>39942.320132845431</v>
+      </c>
+      <c r="F5" s="19">
+        <v>134665.06374812103</v>
+      </c>
+      <c r="G5" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H5" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="19">
+        <v>267262.5158401177</v>
+      </c>
+      <c r="D6" s="19">
+        <v>-79308.845029648743</v>
+      </c>
+      <c r="E6" s="19">
+        <v>-267262.5158401177</v>
+      </c>
+      <c r="F6" s="19">
+        <v>-171206.95707884105</v>
+      </c>
+      <c r="G6" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H6" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.3887761455116625</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="19">
+        <v>232883.63638832315</v>
+      </c>
+      <c r="D7" s="19">
+        <v>232883.63638832315</v>
+      </c>
+      <c r="E7" s="19">
+        <v>152121.692551738</v>
+      </c>
+      <c r="F7" s="19">
+        <v>-83458.466726363054</v>
+      </c>
+      <c r="G7" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H7" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.363227162833111</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="19">
+        <v>344565.84760497557</v>
+      </c>
+      <c r="D8" s="19">
+        <v>-330326.0242480567</v>
+      </c>
+      <c r="E8" s="19">
+        <v>344565.84760497557</v>
+      </c>
+      <c r="F8" s="19">
+        <v>57935.618969373638</v>
+      </c>
+      <c r="G8" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H8" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.2182309774300986</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="19">
+        <v>272960.17044696049</v>
+      </c>
+      <c r="D9" s="19">
+        <v>-225569.23171404022</v>
+      </c>
+      <c r="E9" s="19">
+        <v>272960.17044696049</v>
+      </c>
+      <c r="F9" s="19">
+        <v>-169507.42047289456</v>
+      </c>
+      <c r="G9" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H9" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.1819975885651193</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="19">
+        <v>164726.45662960049</v>
+      </c>
+      <c r="D10" s="19">
+        <v>148657.81471680012</v>
+      </c>
+      <c r="E10" s="19">
+        <v>-151185.92931463249</v>
+      </c>
+      <c r="F10" s="19">
+        <v>23350.003128087439</v>
+      </c>
+      <c r="G10" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H10" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.3128018031641686</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="19">
+        <v>200471.89618848002</v>
+      </c>
+      <c r="D11" s="19">
+        <v>185336.03657680086</v>
+      </c>
+      <c r="E11" s="19">
+        <v>-200471.89618848002</v>
+      </c>
+      <c r="F11" s="19">
+        <v>135105.61813726812</v>
+      </c>
+      <c r="G11" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H11" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.1187865988723222</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="19">
+        <v>420863.91984137846</v>
+      </c>
+      <c r="D12" s="19">
+        <v>299774.33172979916</v>
+      </c>
+      <c r="E12" s="19">
+        <v>25313.229913121555</v>
+      </c>
+      <c r="F12" s="19">
+        <v>-420863.91984137846</v>
+      </c>
+      <c r="G12" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H12" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.382998535558704</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="19">
+        <v>426129.8614656076</v>
+      </c>
+      <c r="D13" s="19">
+        <v>-166170.29089425207</v>
+      </c>
+      <c r="E13" s="19">
+        <v>-426129.8614656076</v>
+      </c>
+      <c r="F13" s="19">
+        <v>-366533.57099260687</v>
+      </c>
+      <c r="G13" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H13" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.2359428504499019</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="19">
+        <v>424465.45475631801</v>
+      </c>
+      <c r="D14" s="19">
+        <v>184504.43087779521</v>
+      </c>
+      <c r="E14" s="19">
+        <v>37589.485224999604</v>
+      </c>
+      <c r="F14" s="19">
+        <v>-240352.91006463554</v>
+      </c>
+      <c r="G14" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H14" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>2.3633417664742749</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="19">
+        <v>407898.88585695246</v>
+      </c>
+      <c r="D15" s="19">
+        <v>-284170.44949149957</v>
+      </c>
+      <c r="E15" s="19">
+        <v>-349868.37987294351</v>
+      </c>
+      <c r="F15" s="19">
+        <v>-407898.88585695246</v>
+      </c>
+      <c r="G15" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H15" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.1406946472669683</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="19">
+        <v>287866.93591597868</v>
+      </c>
+      <c r="D16" s="19">
+        <v>-287866.93591597868</v>
+      </c>
+      <c r="E16" s="19">
+        <v>232965.12259391288</v>
+      </c>
+      <c r="F16" s="19">
+        <v>-166891.5637744788</v>
+      </c>
+      <c r="G16" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H16" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.2047808575836263</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="19">
+        <v>414762.68696002761</v>
+      </c>
+      <c r="D17" s="19">
+        <v>-414762.68696002761</v>
+      </c>
+      <c r="E17" s="19">
+        <v>354572.32206079725</v>
+      </c>
+      <c r="F17" s="19">
+        <v>-231913.01809251832</v>
+      </c>
+      <c r="G17" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H17" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.1892287123512624</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="19">
+        <v>282994.5478730069</v>
+      </c>
+      <c r="D18" s="19">
+        <v>278503.1681062103</v>
+      </c>
+      <c r="E18" s="19">
+        <v>-282994.5478730069</v>
+      </c>
+      <c r="F18" s="19">
+        <v>22014.822838536522</v>
+      </c>
+      <c r="G18" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H18" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.2097999537587358</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="19">
+        <v>478968.65112472116</v>
+      </c>
+      <c r="D19" s="19">
+        <v>478968.65112472116</v>
+      </c>
+      <c r="E19" s="19">
+        <v>-335896.98067721643</v>
+      </c>
+      <c r="F19" s="19">
+        <v>234880.9984710688</v>
+      </c>
+      <c r="G19" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H19" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.2916306594252831</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="19">
+        <v>400383.89722423785</v>
+      </c>
+      <c r="D20" s="19">
+        <v>-198291.45452909271</v>
+      </c>
+      <c r="E20" s="19">
+        <v>165104.22180372407</v>
+      </c>
+      <c r="F20" s="19">
+        <v>-400383.89722423785</v>
+      </c>
+      <c r="G20" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H20" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.4289647373051482</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="19">
+        <v>99253.531037784996</v>
+      </c>
+      <c r="D21" s="19">
+        <v>99253.531037784996</v>
+      </c>
+      <c r="E21" s="19">
+        <v>-94612.714307095623</v>
+      </c>
+      <c r="F21" s="19">
+        <v>-4262.0094475988299</v>
+      </c>
+      <c r="G21" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H21" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.2299107884831475</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="19">
+        <v>189386.51292503346</v>
+      </c>
+      <c r="D22" s="19">
+        <v>65724.887857740279</v>
+      </c>
+      <c r="E22" s="19">
+        <v>-1014.3005179106258</v>
+      </c>
+      <c r="F22" s="19">
+        <v>189386.51292503346</v>
+      </c>
+      <c r="G22" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H22" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.606014828731734</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="19">
+        <v>460723.96871552651</v>
+      </c>
+      <c r="D23" s="19">
+        <v>432001.0085740746</v>
+      </c>
+      <c r="E23" s="19">
+        <v>-345895.68992250971</v>
+      </c>
+      <c r="F23" s="19">
+        <v>460723.96871552651</v>
+      </c>
+      <c r="G23" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H23" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.087678577568266</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="19">
+        <v>486888.6336313393</v>
+      </c>
+      <c r="D24" s="19">
+        <v>328002.53913456807</v>
+      </c>
+      <c r="E24" s="19">
+        <v>486888.6336313393</v>
+      </c>
+      <c r="F24" s="19">
+        <v>-127296.7856583104</v>
+      </c>
+      <c r="G24" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H24" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.3778907800719997</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="19">
+        <v>291128.01861111063</v>
+      </c>
+      <c r="D25" s="19">
+        <v>145176.24855138361</v>
+      </c>
+      <c r="E25" s="19">
+        <v>-288577.03894793586</v>
+      </c>
+      <c r="F25" s="19">
+        <v>291128.01861111063</v>
+      </c>
+      <c r="G25" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H25" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.1380924598092685</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="19">
+        <v>304558.9492679931</v>
+      </c>
+      <c r="D26" s="19">
+        <v>-304558.9492679931</v>
+      </c>
+      <c r="E26" s="19">
+        <v>160938.77382039616</v>
+      </c>
+      <c r="F26" s="19">
+        <v>-64244.352283669519</v>
+      </c>
+      <c r="G26" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H26" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.4775698473112528</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="19">
+        <v>467599.60252829618</v>
+      </c>
+      <c r="D27" s="19">
+        <v>-443804.44126641395</v>
+      </c>
+      <c r="E27" s="19">
+        <v>-310001.00221834274</v>
+      </c>
+      <c r="F27" s="19">
+        <v>427758.76591577532</v>
+      </c>
+      <c r="G27" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H27" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.1521289079241748</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="19">
+        <v>360334.93422578846</v>
+      </c>
+      <c r="D28" s="19">
+        <v>360334.93422578846</v>
+      </c>
+      <c r="E28" s="19">
+        <v>28589.618862812291</v>
+      </c>
+      <c r="F28" s="19">
+        <v>39452.534552828525</v>
+      </c>
+      <c r="G28" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H28" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.6846694717126811</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="19">
+        <v>488651.74208660034</v>
+      </c>
+      <c r="D29" s="19">
+        <v>-488651.74208660034</v>
+      </c>
+      <c r="E29" s="19">
+        <v>-160857.02024646295</v>
+      </c>
+      <c r="F29" s="19">
+        <v>-133634.60678391159</v>
+      </c>
+      <c r="G29" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H29" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.562890694632685</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="19">
+        <v>496791.82729256601</v>
+      </c>
+      <c r="D30" s="19">
+        <v>188432.48757256591</v>
+      </c>
+      <c r="E30" s="19">
+        <v>-496791.82729256601</v>
+      </c>
+      <c r="F30" s="19">
+        <v>-218382.10640544054</v>
+      </c>
+      <c r="G30" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H30" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.4701668085051394</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="19">
+        <v>386503.66287119477</v>
+      </c>
+      <c r="D31" s="19">
+        <v>-350843.66867337201</v>
+      </c>
+      <c r="E31" s="19">
+        <v>-297685.48579161905</v>
+      </c>
+      <c r="F31" s="19">
+        <v>-386503.66287119477</v>
+      </c>
+      <c r="G31" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H31" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.0934350595721805</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="19">
+        <v>457667.0276765849</v>
+      </c>
+      <c r="D32" s="19">
+        <v>457667.0276765849</v>
+      </c>
+      <c r="E32" s="19">
+        <v>-35565.033487819252</v>
+      </c>
+      <c r="F32" s="19">
+        <v>-224249.50559128186</v>
+      </c>
+      <c r="G32" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H32" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.522889732107936</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="19">
+        <v>439645.30654909182</v>
+      </c>
+      <c r="D33" s="19">
+        <v>-279432.17097869067</v>
+      </c>
+      <c r="E33" s="19">
+        <v>-70831.85487798159</v>
+      </c>
+      <c r="F33" s="19">
+        <v>-246607.69302283702</v>
+      </c>
+      <c r="G33" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H33" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.9701467055318678</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="19">
+        <v>393074.74460657197</v>
+      </c>
+      <c r="D34" s="19">
+        <v>56393.642115526716</v>
+      </c>
+      <c r="E34" s="19">
+        <v>223976.80436867545</v>
+      </c>
+      <c r="F34" s="19">
+        <v>393074.74460657197</v>
+      </c>
+      <c r="G34" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H34" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.4657006483798154</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="19">
+        <v>90378.162333960994</v>
+      </c>
+      <c r="D35" s="19">
+        <v>28545.707702202024</v>
+      </c>
+      <c r="E35" s="19">
+        <v>42575.182998143253</v>
+      </c>
+      <c r="F35" s="19">
+        <v>90378.162333960994</v>
+      </c>
+      <c r="G35" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H35" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.4787225818066949</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="19">
+        <v>393285.67029121844</v>
+      </c>
+      <c r="D36" s="19">
+        <v>-35499.525182949204</v>
+      </c>
+      <c r="E36" s="19">
+        <v>34780.54477595014</v>
+      </c>
+      <c r="F36" s="19">
+        <v>-149941.29345645913</v>
+      </c>
+      <c r="G36" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H36" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="19">
+        <v>440848.83256897033</v>
+      </c>
+      <c r="D37" s="19">
+        <v>-214386.70166716166</v>
+      </c>
+      <c r="E37" s="19">
+        <v>-440848.83256897033</v>
+      </c>
+      <c r="F37" s="19">
+        <v>165646.9745007524</v>
+      </c>
+      <c r="G37" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H37" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.4483558531565801</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="19">
+        <v>328920.13906211406</v>
+      </c>
+      <c r="D38" s="19">
+        <v>190844.66829319741</v>
+      </c>
+      <c r="E38" s="19">
+        <v>328920.13906211406</v>
+      </c>
+      <c r="F38" s="19">
+        <v>232781.43882957986</v>
+      </c>
+      <c r="G38" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H38" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.2541055741482667</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="19">
+        <v>456774.86950109643</v>
+      </c>
+      <c r="D39" s="19">
+        <v>456774.86950109643</v>
+      </c>
+      <c r="E39" s="19">
+        <v>-231484.79071704322</v>
+      </c>
+      <c r="F39" s="19">
+        <v>425410.9160455619</v>
+      </c>
+      <c r="G39" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H39" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.1664061708913509</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="19">
+        <v>412963.79622878722</v>
+      </c>
+      <c r="D40" s="19">
+        <v>-189878.20673391665</v>
+      </c>
+      <c r="E40" s="19">
+        <v>-396210.44774176471</v>
+      </c>
+      <c r="F40" s="19">
+        <v>-412963.79622878722</v>
+      </c>
+      <c r="G40" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H40" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.1642964317010327</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="19">
+        <v>401556.07866690296</v>
+      </c>
+      <c r="D41" s="19">
+        <v>-125863.94394665578</v>
+      </c>
+      <c r="E41" s="19">
+        <v>141539.07658195542</v>
+      </c>
+      <c r="F41" s="19">
+        <v>-364550.94305091596</v>
+      </c>
+      <c r="G41" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H41" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.6616684375706057</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="19">
+        <v>461275.96682282712</v>
+      </c>
+      <c r="D42" s="19">
+        <v>-191055.25599598314</v>
+      </c>
+      <c r="E42" s="19">
+        <v>461275.96682282712</v>
+      </c>
+      <c r="F42" s="19">
+        <v>-444435.3682748655</v>
+      </c>
+      <c r="G42" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H42" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.1731484210080103</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="19">
+        <v>465964.98751160642</v>
+      </c>
+      <c r="D43" s="19">
+        <v>361255.80330106954</v>
+      </c>
+      <c r="E43" s="19">
+        <v>-116695.34114464809</v>
+      </c>
+      <c r="F43" s="19">
+        <v>187596.62736927171</v>
+      </c>
+      <c r="G43" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H43" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.8706503584274858</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="19">
+        <v>485649.32087850187</v>
+      </c>
+      <c r="D44" s="19">
+        <v>-280687.90206773556</v>
+      </c>
+      <c r="E44" s="19">
+        <v>485649.32087850187</v>
+      </c>
+      <c r="F44" s="19">
+        <v>-229443.34130623878</v>
+      </c>
+      <c r="G44" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H44" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.3622913156759073</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="19">
+        <v>269757.60639827582</v>
+      </c>
+      <c r="D45" s="19">
+        <v>269757.60639827582</v>
+      </c>
+      <c r="E45" s="19">
+        <v>44876.016883783625</v>
+      </c>
+      <c r="F45" s="19">
+        <v>253478.62617432908</v>
+      </c>
+      <c r="G45" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H45" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.2298762909230818</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="19">
+        <v>276626.51726431295</v>
+      </c>
+      <c r="D46" s="19">
+        <v>145843.99946442444</v>
+      </c>
+      <c r="E46" s="19">
+        <v>276626.51726431295</v>
+      </c>
+      <c r="F46" s="19">
+        <v>-123989.86240828148</v>
+      </c>
+      <c r="G46" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H46" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.3979266569721569</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="19">
+        <v>430286.03354892012</v>
+      </c>
+      <c r="D47" s="19">
+        <v>49316.557022188674</v>
+      </c>
+      <c r="E47" s="19">
+        <v>395936.85287168692</v>
+      </c>
+      <c r="F47" s="19">
+        <v>-430286.03354892012</v>
+      </c>
+      <c r="G47" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H47" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.2465502624628073</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" s="19">
+        <v>485566.31592848164</v>
+      </c>
+      <c r="D48" s="19">
+        <v>-366315.58531614952</v>
+      </c>
+      <c r="E48" s="19">
+        <v>-252988.97761278704</v>
+      </c>
+      <c r="F48" s="19">
+        <v>305971.24461556715</v>
+      </c>
+      <c r="G48" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H48" s="20">
+        <f>MIN((1.7*tblalpha_m[[#This Row],[Mmax]])/SQRT(tblalpha_m[[#This Row],[M2]]^2+tblalpha_m[[#This Row],[M3]]^2+tblalpha_m[[#This Row],[M4]]^2),2.5)</f>
+        <v>1.5280873538617674</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="2" t="str">
+        <f t="array" ref="B50:B75">TRANSPOSE(tblalpha_m[#Headers])</f>
+        <v>Section</v>
+      </c>
+      <c r="C50" s="4" t="str">
+        <f t="array" aca="1" ref="C50" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B50&amp;"]")&lt;&gt;"","'"&amp;TEXT(INDIRECT("tblalpha_m["&amp;B50&amp;"]"),"0.00000E+00")&amp;"', ",""))</f>
+        <v xml:space="preserve">'45x45x3EA', '150x150x12EA', '310UC137', '75x50x8UA', '700WB173', '800WB168', '400WC181', '200x200x26EA', '310UB40.4', '310UC158', '40x40x6EA', '1200WB342', '180UB18.1', '500WC267', '200UBP146', '65x65x8EA', '250UBP62.6', '25x25x5EA', '300PFC', '350WC280', '310UC118', '125x125x12EA', '125x75x12UA', '250UB25.7', '250UBP84.9', '100x100x12EA', '65x50x8UA', '150PFC', '200PFC', '250UC72.9', '310UC96.8', '400WC144', '45x45x5EA', '400WC328', '610UB125', '75x75x10EA', '200UB18.2', '200x200x20EA', '65x50x5UA', '800WB122', '75x50x5UA', '100x100x8EA', '125TFB', '1200WB455', '310UB46.2', '75x75x6EA', </v>
+      </c>
+      <c r="D50" s="2" t="str">
+        <f ca="1">B50&amp;" = ("&amp;LEFT(C50,LEN(C50)-2)&amp;")"</f>
+        <v>Section = ('45x45x3EA', '150x150x12EA', '310UC137', '75x50x8UA', '700WB173', '800WB168', '400WC181', '200x200x26EA', '310UB40.4', '310UC158', '40x40x6EA', '1200WB342', '180UB18.1', '500WC267', '200UBP146', '65x65x8EA', '250UBP62.6', '25x25x5EA', '300PFC', '350WC280', '310UC118', '125x125x12EA', '125x75x12UA', '250UB25.7', '250UBP84.9', '100x100x12EA', '65x50x8UA', '150PFC', '200PFC', '250UC72.9', '310UC96.8', '400WC144', '45x45x5EA', '400WC328', '610UB125', '75x75x10EA', '200UB18.2', '200x200x20EA', '65x50x5UA', '800WB122', '75x50x5UA', '100x100x8EA', '125TFB', '1200WB455', '310UB46.2', '75x75x6EA')</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B51" s="2" t="str">
+        <v>Mmax</v>
+      </c>
+      <c r="C51" s="4" t="str">
+        <f t="array" aca="1" ref="C51" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B51&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B51&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">4.67469E+05, 3.49510E+05, 3.47664E+05, 2.67263E+05, 2.32884E+05, 3.44566E+05, 2.72960E+05, 1.64726E+05, 2.00472E+05, 4.20864E+05, 4.26130E+05, 4.24465E+05, 4.07899E+05, 2.87867E+05, 4.14763E+05, 2.82995E+05, 4.78969E+05, 4.00384E+05, 9.92535E+04, 1.89387E+05, 4.60724E+05, 4.86889E+05, 2.91128E+05, 3.04559E+05, 4.67600E+05, 3.60335E+05, 4.88652E+05, 4.96792E+05, 3.86504E+05, 4.57667E+05, 4.39645E+05, 3.93075E+05, 9.03782E+04, 3.93286E+05, 4.40849E+05, 3.28920E+05, 4.56775E+05, 4.12964E+05, 4.01556E+05, 4.61276E+05, 4.65965E+05, 4.85649E+05, 2.69758E+05, 2.76627E+05, 4.30286E+05, 4.85566E+05, </v>
+      </c>
+      <c r="D51" s="2" t="str">
+        <f t="shared" ref="D51:D75" ca="1" si="0">B51&amp;" = ("&amp;LEFT(C51,LEN(C51)-2)&amp;")"</f>
+        <v>Mmax = (4.67469E+05, 3.49510E+05, 3.47664E+05, 2.67263E+05, 2.32884E+05, 3.44566E+05, 2.72960E+05, 1.64726E+05, 2.00472E+05, 4.20864E+05, 4.26130E+05, 4.24465E+05, 4.07899E+05, 2.87867E+05, 4.14763E+05, 2.82995E+05, 4.78969E+05, 4.00384E+05, 9.92535E+04, 1.89387E+05, 4.60724E+05, 4.86889E+05, 2.91128E+05, 3.04559E+05, 4.67600E+05, 3.60335E+05, 4.88652E+05, 4.96792E+05, 3.86504E+05, 4.57667E+05, 4.39645E+05, 3.93075E+05, 9.03782E+04, 3.93286E+05, 4.40849E+05, 3.28920E+05, 4.56775E+05, 4.12964E+05, 4.01556E+05, 4.61276E+05, 4.65965E+05, 4.85649E+05, 2.69758E+05, 2.76627E+05, 4.30286E+05, 4.85566E+05)</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="2" t="str">
+        <v>M2</v>
+      </c>
+      <c r="C52" s="4" t="str">
+        <f t="array" aca="1" ref="C52" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B52&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B52&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">-4.67469E+05, -1.42941E+05, 3.37893E+04, -7.93088E+04, 2.32884E+05, -3.30326E+05, -2.25569E+05, 1.48658E+05, 1.85336E+05, 2.99774E+05, -1.66170E+05, 1.84504E+05, -2.84170E+05, -2.87867E+05, -4.14763E+05, 2.78503E+05, 4.78969E+05, -1.98291E+05, 9.92535E+04, 6.57249E+04, 4.32001E+05, 3.28003E+05, 1.45176E+05, -3.04559E+05, -4.43804E+05, 3.60335E+05, -4.88652E+05, 1.88432E+05, -3.50844E+05, 4.57667E+05, -2.79432E+05, 5.63936E+04, 2.85457E+04, -3.54995E+04, -2.14387E+05, 1.90845E+05, 4.56775E+05, -1.89878E+05, -1.25864E+05, -1.91055E+05, 3.61256E+05, -2.80688E+05, 2.69758E+05, 1.45844E+05, 4.93166E+04, -3.66316E+05, </v>
+      </c>
+      <c r="D52" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>M2 = (-4.67469E+05, -1.42941E+05, 3.37893E+04, -7.93088E+04, 2.32884E+05, -3.30326E+05, -2.25569E+05, 1.48658E+05, 1.85336E+05, 2.99774E+05, -1.66170E+05, 1.84504E+05, -2.84170E+05, -2.87867E+05, -4.14763E+05, 2.78503E+05, 4.78969E+05, -1.98291E+05, 9.92535E+04, 6.57249E+04, 4.32001E+05, 3.28003E+05, 1.45176E+05, -3.04559E+05, -4.43804E+05, 3.60335E+05, -4.88652E+05, 1.88432E+05, -3.50844E+05, 4.57667E+05, -2.79432E+05, 5.63936E+04, 2.85457E+04, -3.54995E+04, -2.14387E+05, 1.90845E+05, 4.56775E+05, -1.89878E+05, -1.25864E+05, -1.91055E+05, 3.61256E+05, -2.80688E+05, 2.69758E+05, 1.45844E+05, 4.93166E+04, -3.66316E+05)</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" s="2" t="str">
+        <v>M3</v>
+      </c>
+      <c r="C53" s="4" t="str">
+        <f t="array" aca="1" ref="C53" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B53&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B53&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">3.09832E+05, 3.49510E+05, 3.99423E+04, -2.67263E+05, 1.52122E+05, 3.44566E+05, 2.72960E+05, -1.51186E+05, -2.00472E+05, 2.53132E+04, -4.26130E+05, 3.75895E+04, -3.49868E+05, 2.32965E+05, 3.54572E+05, -2.82995E+05, -3.35897E+05, 1.65104E+05, -9.46127E+04, -1.01430E+03, -3.45896E+05, 4.86889E+05, -2.88577E+05, 1.60939E+05, -3.10001E+05, 2.85896E+04, -1.60857E+05, -4.96792E+05, -2.97685E+05, -3.55650E+04, -7.08319E+04, 2.23977E+05, 4.25752E+04, 3.47805E+04, -4.40849E+05, 3.28920E+05, -2.31485E+05, -3.96210E+05, 1.41539E+05, 4.61276E+05, -1.16695E+05, 4.85649E+05, 4.48760E+04, 2.76627E+05, 3.95937E+05, -2.52989E+05, </v>
+      </c>
+      <c r="D53" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>M3 = (3.09832E+05, 3.49510E+05, 3.99423E+04, -2.67263E+05, 1.52122E+05, 3.44566E+05, 2.72960E+05, -1.51186E+05, -2.00472E+05, 2.53132E+04, -4.26130E+05, 3.75895E+04, -3.49868E+05, 2.32965E+05, 3.54572E+05, -2.82995E+05, -3.35897E+05, 1.65104E+05, -9.46127E+04, -1.01430E+03, -3.45896E+05, 4.86889E+05, -2.88577E+05, 1.60939E+05, -3.10001E+05, 2.85896E+04, -1.60857E+05, -4.96792E+05, -2.97685E+05, -3.55650E+04, -7.08319E+04, 2.23977E+05, 4.25752E+04, 3.47805E+04, -4.40849E+05, 3.28920E+05, -2.31485E+05, -3.96210E+05, 1.41539E+05, 4.61276E+05, -1.16695E+05, 4.85649E+05, 4.48760E+04, 2.76627E+05, 3.95937E+05, -2.52989E+05)</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B54" s="2" t="str">
+        <v>M4</v>
+      </c>
+      <c r="C54" s="4" t="str">
+        <f t="array" aca="1" ref="C54" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B54&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B54&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">-3.67540E+05, -2.72333E+05, 1.34665E+05, -1.71207E+05, -8.34585E+04, 5.79356E+04, -1.69507E+05, 2.33500E+04, 1.35106E+05, -4.20864E+05, -3.66534E+05, -2.40353E+05, -4.07899E+05, -1.66892E+05, -2.31913E+05, 2.20148E+04, 2.34881E+05, -4.00384E+05, -4.26201E+03, 1.89387E+05, 4.60724E+05, -1.27297E+05, 2.91128E+05, -6.42444E+04, 4.27759E+05, 3.94525E+04, -1.33635E+05, -2.18382E+05, -3.86504E+05, -2.24250E+05, -2.46608E+05, 3.93075E+05, 9.03782E+04, -1.49941E+05, 1.65647E+05, 2.32781E+05, 4.25411E+05, -4.12964E+05, -3.64551E+05, -4.44435E+05, 1.87597E+05, -2.29443E+05, 2.53479E+05, -1.23990E+05, -4.30286E+05, 3.05971E+05, </v>
+      </c>
+      <c r="D54" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>M4 = (-3.67540E+05, -2.72333E+05, 1.34665E+05, -1.71207E+05, -8.34585E+04, 5.79356E+04, -1.69507E+05, 2.33500E+04, 1.35106E+05, -4.20864E+05, -3.66534E+05, -2.40353E+05, -4.07899E+05, -1.66892E+05, -2.31913E+05, 2.20148E+04, 2.34881E+05, -4.00384E+05, -4.26201E+03, 1.89387E+05, 4.60724E+05, -1.27297E+05, 2.91128E+05, -6.42444E+04, 4.27759E+05, 3.94525E+04, -1.33635E+05, -2.18382E+05, -3.86504E+05, -2.24250E+05, -2.46608E+05, 3.93075E+05, 9.03782E+04, -1.49941E+05, 1.65647E+05, 2.32781E+05, 4.25411E+05, -4.12964E+05, -3.64551E+05, -4.44435E+05, 1.87597E+05, -2.29443E+05, 2.53479E+05, -1.23990E+05, -4.30286E+05, 3.05971E+05)</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="2" t="str">
+        <v>αm_max</v>
+      </c>
+      <c r="C55" s="4" t="str">
+        <f t="array" aca="1" ref="C55" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B55&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B55&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, </v>
+      </c>
+      <c r="D55" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>αm_max = (2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00, 2.50000E+00)</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B56" s="2" t="str">
+        <v>αm</v>
+      </c>
+      <c r="C56" s="4" t="str">
+        <f t="array" aca="1" ref="C56" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B56&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B56&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v xml:space="preserve">1.18518E+00, 1.27622E+00, 2.50000E+00, 1.38878E+00, 1.36323E+00, 1.21823E+00, 1.18200E+00, 1.31280E+00, 1.11879E+00, 1.38300E+00, 1.23594E+00, 2.36334E+00, 1.14069E+00, 1.20478E+00, 1.18923E+00, 1.20980E+00, 1.29163E+00, 1.42896E+00, 1.22991E+00, 1.60601E+00, 1.08768E+00, 1.37789E+00, 1.13809E+00, 1.47757E+00, 1.15213E+00, 1.68467E+00, 1.56289E+00, 1.47017E+00, 1.09344E+00, 1.52289E+00, 1.97015E+00, 1.46570E+00, 1.47872E+00, 2.50000E+00, 1.44836E+00, 1.25411E+00, 1.16641E+00, 1.16430E+00, 1.66167E+00, 1.17315E+00, 1.87065E+00, 1.36229E+00, 1.22988E+00, 1.39793E+00, 1.24655E+00, 1.52809E+00, </v>
+      </c>
+      <c r="D56" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>αm = (1.18518E+00, 1.27622E+00, 2.50000E+00, 1.38878E+00, 1.36323E+00, 1.21823E+00, 1.18200E+00, 1.31280E+00, 1.11879E+00, 1.38300E+00, 1.23594E+00, 2.36334E+00, 1.14069E+00, 1.20478E+00, 1.18923E+00, 1.20980E+00, 1.29163E+00, 1.42896E+00, 1.22991E+00, 1.60601E+00, 1.08768E+00, 1.37789E+00, 1.13809E+00, 1.47757E+00, 1.15213E+00, 1.68467E+00, 1.56289E+00, 1.47017E+00, 1.09344E+00, 1.52289E+00, 1.97015E+00, 1.46570E+00, 1.47872E+00, 2.50000E+00, 1.44836E+00, 1.25411E+00, 1.16641E+00, 1.16430E+00, 1.66167E+00, 1.17315E+00, 1.87065E+00, 1.36229E+00, 1.22988E+00, 1.39793E+00, 1.24655E+00, 1.52809E+00)</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B57" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C57" s="4" t="e">
+        <f t="array" aca="1" ref="C57" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B57&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B57&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D57" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B58" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C58" s="4" t="e">
+        <f t="array" aca="1" ref="C58" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B58&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B58&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D58" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B59" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C59" s="4" t="e">
+        <f t="array" aca="1" ref="C59" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B59&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B59&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D59" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B60" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C60" s="4" t="e">
+        <f t="array" aca="1" ref="C60" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B60&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B60&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D60" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B61" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C61" s="4" t="e">
+        <f t="array" aca="1" ref="C61" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B61&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B61&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D61" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B62" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C62" s="4" t="e">
+        <f t="array" aca="1" ref="C62" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B62&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B62&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D62" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B63" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C63" s="4" t="e">
+        <f t="array" aca="1" ref="C63" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B63&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B63&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D63" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B64" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C64" s="4" t="e">
+        <f t="array" aca="1" ref="C64" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B64&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B64&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D64" s="2" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="e">
         <v>#N/A</v>
       </c>
       <c r="C65" s="4" t="e">
-        <f t="array" aca="1" ref="C65" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B65&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B65&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <f t="array" aca="1" ref="C65" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B65&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B65&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D65" s="2" t="e">
@@ -5673,7 +7975,7 @@
         <v>#N/A</v>
       </c>
       <c r="C66" s="4" t="e">
-        <f t="array" aca="1" ref="C66" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B66&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B66&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <f t="array" aca="1" ref="C66" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B66&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B66&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D66" s="2" t="e">
@@ -5686,7 +7988,7 @@
         <v>#N/A</v>
       </c>
       <c r="C67" s="4" t="e">
-        <f t="array" aca="1" ref="C67" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B67&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B67&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <f t="array" aca="1" ref="C67" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B67&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B67&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D67" s="2" t="e">
@@ -5699,7 +8001,7 @@
         <v>#N/A</v>
       </c>
       <c r="C68" s="4" t="e">
-        <f t="array" aca="1" ref="C68" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B68&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B68&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <f t="array" aca="1" ref="C68" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B68&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B68&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D68" s="2" t="e">
@@ -5712,7 +8014,7 @@
         <v>#N/A</v>
       </c>
       <c r="C69" s="4" t="e">
-        <f t="array" aca="1" ref="C69" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B69&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B69&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <f t="array" aca="1" ref="C69" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B69&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B69&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D69" s="2" t="e">
@@ -5725,7 +8027,7 @@
         <v>#N/A</v>
       </c>
       <c r="C70" s="4" t="e">
-        <f t="array" aca="1" ref="C70" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B70&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B70&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <f t="array" aca="1" ref="C70" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B70&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B70&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D70" s="2" t="e">
@@ -5738,7 +8040,7 @@
         <v>#N/A</v>
       </c>
       <c r="C71" s="4" t="e">
-        <f t="array" aca="1" ref="C71" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B71&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B71&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <f t="array" aca="1" ref="C71" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B71&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B71&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D71" s="2" t="e">
@@ -5751,7 +8053,7 @@
         <v>#N/A</v>
       </c>
       <c r="C72" s="4" t="e">
-        <f t="array" aca="1" ref="C72" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B72&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B72&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <f t="array" aca="1" ref="C72" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B72&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B72&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D72" s="2" t="e">
@@ -5764,7 +8066,7 @@
         <v>#N/A</v>
       </c>
       <c r="C73" s="4" t="e">
-        <f t="array" aca="1" ref="C73" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B73&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B73&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <f t="array" aca="1" ref="C73" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B73&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B73&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D73" s="2" t="e">
@@ -5777,7 +8079,7 @@
         <v>#N/A</v>
       </c>
       <c r="C74" s="4" t="e">
-        <f t="array" aca="1" ref="C74" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B74&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B74&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <f t="array" aca="1" ref="C74" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B74&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B74&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D74" s="2" t="e">
@@ -5790,7 +8092,7 @@
         <v>#N/A</v>
       </c>
       <c r="C75" s="4" t="e">
-        <f t="array" aca="1" ref="C75" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblM_o["&amp;B75&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblM_o["&amp;B75&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
+        <f t="array" aca="1" ref="C75" ca="1">_xlfn.CONCAT(IF(INDIRECT("tblalpha_m["&amp;B75&amp;"]")&lt;&gt;"",TEXT(INDIRECT("tblalpha_m["&amp;B75&amp;"]"),"0.00000E+00")&amp;", ","0E+0, "))</f>
         <v>#N/A</v>
       </c>
       <c r="D75" s="2" t="e">

</xml_diff>